<commit_message>
added template types for diff languages
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP_REPO\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4657306-45D8-4171-BCB8-81A9120007C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="3150" yWindow="3150" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3652" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3724" uniqueCount="314">
   <si>
     <t>lang_code</t>
   </si>
@@ -951,12 +952,30 @@
   </si>
   <si>
     <t>Template for Acknowledgement in Android regclient</t>
+  </si>
+  <si>
+    <t>tnc-order-a-physical-card</t>
+  </si>
+  <si>
+    <t>Order a physical card</t>
+  </si>
+  <si>
+    <t>tnc-share-cred-with-partner</t>
+  </si>
+  <si>
+    <t>Share your credential with a partner</t>
+  </si>
+  <si>
+    <t>tnc-update-demo</t>
+  </si>
+  <si>
+    <t>Update demographic data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1046,7 +1065,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1324,11 +1343,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D951"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A900" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A902" sqref="A902:D913"/>
+    <sheetView tabSelected="1" topLeftCell="A916" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C934" sqref="C934"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14121,96 +14140,294 @@
       </c>
     </row>
     <row r="914" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A914" s="4"/>
+      <c r="A914" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B914" t="s">
+        <v>308</v>
+      </c>
+      <c r="C914" t="s">
+        <v>309</v>
+      </c>
+      <c r="D914" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="915" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A915" s="4"/>
+      <c r="A915" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B915" t="s">
+        <v>308</v>
+      </c>
+      <c r="C915" t="s">
+        <v>309</v>
+      </c>
+      <c r="D915" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="916" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A916" s="4"/>
+      <c r="A916" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B916" t="s">
+        <v>308</v>
+      </c>
+      <c r="C916" t="s">
+        <v>309</v>
+      </c>
+      <c r="D916" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="917" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A917" s="4"/>
+      <c r="A917" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B917" t="s">
+        <v>308</v>
+      </c>
+      <c r="C917" t="s">
+        <v>309</v>
+      </c>
+      <c r="D917" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="918" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A918" s="4"/>
+      <c r="A918" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B918" t="s">
+        <v>308</v>
+      </c>
+      <c r="C918" t="s">
+        <v>309</v>
+      </c>
+      <c r="D918" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="919" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A919" s="4"/>
+      <c r="A919" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B919" t="s">
+        <v>308</v>
+      </c>
+      <c r="C919" t="s">
+        <v>309</v>
+      </c>
+      <c r="D919" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="920" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A920" s="4"/>
+      <c r="A920" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B920" t="s">
+        <v>310</v>
+      </c>
+      <c r="C920" t="s">
+        <v>311</v>
+      </c>
+      <c r="D920" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="921" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A921" s="4"/>
+      <c r="A921" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B921" t="s">
+        <v>310</v>
+      </c>
+      <c r="C921" t="s">
+        <v>311</v>
+      </c>
+      <c r="D921" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="922" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A922" s="4"/>
+      <c r="A922" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B922" t="s">
+        <v>310</v>
+      </c>
+      <c r="C922" t="s">
+        <v>311</v>
+      </c>
+      <c r="D922" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="923" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A923" s="4"/>
+      <c r="A923" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B923" t="s">
+        <v>310</v>
+      </c>
+      <c r="C923" t="s">
+        <v>311</v>
+      </c>
+      <c r="D923" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="924" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A924" s="4"/>
+      <c r="A924" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B924" t="s">
+        <v>310</v>
+      </c>
+      <c r="C924" t="s">
+        <v>311</v>
+      </c>
+      <c r="D924" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="925" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A925" s="4"/>
+      <c r="A925" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B925" t="s">
+        <v>310</v>
+      </c>
+      <c r="C925" t="s">
+        <v>311</v>
+      </c>
+      <c r="D925" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="926" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A926" s="4"/>
+      <c r="A926" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B926" t="s">
+        <v>312</v>
+      </c>
+      <c r="C926" t="s">
+        <v>313</v>
+      </c>
+      <c r="D926" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="927" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A927" s="4"/>
+      <c r="A927" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B927" t="s">
+        <v>312</v>
+      </c>
+      <c r="C927" t="s">
+        <v>313</v>
+      </c>
+      <c r="D927" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="928" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A928" s="4"/>
-    </row>
-    <row r="929" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A929" s="4"/>
-    </row>
-    <row r="930" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A930" s="4"/>
-    </row>
-    <row r="931" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A931" s="4"/>
-    </row>
-    <row r="932" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A928" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B928" t="s">
+        <v>312</v>
+      </c>
+      <c r="C928" t="s">
+        <v>313</v>
+      </c>
+      <c r="D928" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="929" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A929" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B929" t="s">
+        <v>312</v>
+      </c>
+      <c r="C929" t="s">
+        <v>313</v>
+      </c>
+      <c r="D929" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="930" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A930" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B930" t="s">
+        <v>312</v>
+      </c>
+      <c r="C930" t="s">
+        <v>313</v>
+      </c>
+      <c r="D930" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="931" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A931" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B931" t="s">
+        <v>312</v>
+      </c>
+      <c r="C931" t="s">
+        <v>313</v>
+      </c>
+      <c r="D931" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="932" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A932" s="4"/>
     </row>
-    <row r="933" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="933" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A933" s="4"/>
     </row>
-    <row r="934" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="934" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A934" s="4"/>
     </row>
-    <row r="935" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="935" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A935" s="4"/>
     </row>
-    <row r="936" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="936" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A936" s="4"/>
     </row>
-    <row r="937" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A937" s="4"/>
     </row>
-    <row r="938" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="938" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A938" s="4"/>
     </row>
-    <row r="939" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A939" s="4"/>
     </row>
-    <row r="940" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A940" s="4"/>
     </row>
-    <row r="941" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A941" s="4"/>
     </row>
-    <row r="942" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A942" s="4"/>
     </row>
-    <row r="943" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A943" s="4"/>
     </row>
-    <row r="944" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A944" s="4"/>
     </row>
     <row r="945" spans="1:1" x14ac:dyDescent="0.25">
@@ -14235,7 +14452,7 @@
       <c r="A951" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D400"/>
+  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
added templates for email notification
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4657306-45D8-4171-BCB8-81A9120007C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78468D9C-5FFE-4353-AB34-76DE9A0DD193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="3150" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3724" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4880" uniqueCount="412">
   <si>
     <t>lang_code</t>
   </si>
@@ -970,6 +970,300 @@
   </si>
   <si>
     <t>Update demographic data</t>
+  </si>
+  <si>
+    <t>Success email to customize and download my card</t>
+  </si>
+  <si>
+    <t>Failure email to customize and download my card</t>
+  </si>
+  <si>
+    <t>Request received email to customize and download my card</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-request-received-email-content</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-success-email-content</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-failure-email-content</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>Request received email subject to customize and download my card</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-success-email-subject</t>
+  </si>
+  <si>
+    <t>Success email subject to customize and download my card</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-failure-email-subject</t>
+  </si>
+  <si>
+    <t>Failure email subject to customize and download my card</t>
+  </si>
+  <si>
+    <t>Request received email subject to order a physical card</t>
+  </si>
+  <si>
+    <t>Success email subject to order a physical card</t>
+  </si>
+  <si>
+    <t>Failure email subject to order a physical card</t>
+  </si>
+  <si>
+    <t>Request received email to order a physical card</t>
+  </si>
+  <si>
+    <t>Success email to order a physical card</t>
+  </si>
+  <si>
+    <t>Failure email to order a physical card</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-success-email-subject</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-failure-email-subject</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-request-received-email-content</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-success-email-content</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-failure-email-content</t>
+  </si>
+  <si>
+    <t>Request received email subject to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Success email subject to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Failure email subject to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Request received email to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Success email to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Failure email to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-success-email-subject</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-failure-email-subject</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-request-received-email-content</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-success-email-content</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-failure-email-content</t>
+  </si>
+  <si>
+    <t>Request received email subject to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Success email subject to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Failure email subject to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Request received email to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Success email to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Failure email to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-success-email-subject</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-failure-email-subject</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-request-received-email-content</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-success-email-content</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-failure-email-content</t>
+  </si>
+  <si>
+    <t>Request received email subject to self update demographic data</t>
+  </si>
+  <si>
+    <t>Success email subject to self update demographic data</t>
+  </si>
+  <si>
+    <t>Failure email subject to self update demographic data</t>
+  </si>
+  <si>
+    <t>Request received email to self update demographic data</t>
+  </si>
+  <si>
+    <t>Success email to self update demographic data</t>
+  </si>
+  <si>
+    <t>Failure email to self update demographic data</t>
+  </si>
+  <si>
+    <t>update-demo-data-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>update-demo-data-success-email-subject</t>
+  </si>
+  <si>
+    <t>update-demo-data-failure-email-subject</t>
+  </si>
+  <si>
+    <t>update-demo-data-request-received-email-content</t>
+  </si>
+  <si>
+    <t>update-demo-data-success-email-content</t>
+  </si>
+  <si>
+    <t>update-demo-data-failure-email-content</t>
+  </si>
+  <si>
+    <t>Request received email subject to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Success email subject to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Failure email subject to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Request received email to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Success email to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Failure email to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-success-email-subject</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-failure-email-subject</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-request-received-email-content</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-success-email-content</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-failure-email-content</t>
+  </si>
+  <si>
+    <t>Request received email subject to get my UIN card</t>
+  </si>
+  <si>
+    <t>Success email subject to get my UIN card</t>
+  </si>
+  <si>
+    <t>Failure email subject to get my UIN card</t>
+  </si>
+  <si>
+    <t>Request received email to get my UIN card</t>
+  </si>
+  <si>
+    <t>Success email to get my UIN card</t>
+  </si>
+  <si>
+    <t>Failure email to get my UIN card</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-success-email-subject</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-failure-email-subject</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-request-received-email-content</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-success-email-content</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-failure-email-content</t>
+  </si>
+  <si>
+    <t>Request received email subject to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Success email subject to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Failure email subject to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Request received email to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Success email to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Failure email to verify my phone and email</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-success-email-subject</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-failure-email-subject</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-request-received-email-content</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-success-email-content</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-failure-email-content</t>
+  </si>
+  <si>
+    <t>Acknowledgement for share credential with a partner</t>
+  </si>
+  <si>
+    <t>acknowledgement-share-cred-with-partner</t>
   </si>
 </sst>
 </file>
@@ -1344,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D951"/>
+  <dimension ref="A1:D1220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A916" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C934" sqref="C934"/>
+    <sheetView tabSelected="1" topLeftCell="A1212" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1223" sqref="C1223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14392,64 +14686,4050 @@
       </c>
     </row>
     <row r="932" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A932" s="4"/>
+      <c r="A932" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B932" t="s">
+        <v>320</v>
+      </c>
+      <c r="C932" t="s">
+        <v>321</v>
+      </c>
+      <c r="D932" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="933" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A933" s="4"/>
+      <c r="A933" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B933" t="s">
+        <v>320</v>
+      </c>
+      <c r="C933" t="s">
+        <v>321</v>
+      </c>
+      <c r="D933" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="934" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A934" s="4"/>
+      <c r="A934" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B934" t="s">
+        <v>320</v>
+      </c>
+      <c r="C934" t="s">
+        <v>321</v>
+      </c>
+      <c r="D934" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="935" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A935" s="4"/>
+      <c r="A935" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B935" t="s">
+        <v>320</v>
+      </c>
+      <c r="C935" t="s">
+        <v>321</v>
+      </c>
+      <c r="D935" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="936" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A936" s="4"/>
+      <c r="A936" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B936" t="s">
+        <v>320</v>
+      </c>
+      <c r="C936" t="s">
+        <v>321</v>
+      </c>
+      <c r="D936" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="937" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A937" s="4"/>
+      <c r="A937" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B937" t="s">
+        <v>320</v>
+      </c>
+      <c r="C937" t="s">
+        <v>321</v>
+      </c>
+      <c r="D937" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="938" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A938" s="4"/>
+      <c r="A938" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B938" t="s">
+        <v>322</v>
+      </c>
+      <c r="C938" t="s">
+        <v>323</v>
+      </c>
+      <c r="D938" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="939" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A939" s="4"/>
+      <c r="A939" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B939" t="s">
+        <v>322</v>
+      </c>
+      <c r="C939" t="s">
+        <v>323</v>
+      </c>
+      <c r="D939" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="940" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A940" s="4"/>
+      <c r="A940" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B940" t="s">
+        <v>322</v>
+      </c>
+      <c r="C940" t="s">
+        <v>323</v>
+      </c>
+      <c r="D940" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="941" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A941" s="4"/>
+      <c r="A941" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B941" t="s">
+        <v>322</v>
+      </c>
+      <c r="C941" t="s">
+        <v>323</v>
+      </c>
+      <c r="D941" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="942" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A942" s="4"/>
+      <c r="A942" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B942" t="s">
+        <v>322</v>
+      </c>
+      <c r="C942" t="s">
+        <v>323</v>
+      </c>
+      <c r="D942" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="943" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A943" s="4"/>
+      <c r="A943" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B943" t="s">
+        <v>322</v>
+      </c>
+      <c r="C943" t="s">
+        <v>323</v>
+      </c>
+      <c r="D943" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="944" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A944" s="4"/>
-    </row>
-    <row r="945" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A945" s="4"/>
-    </row>
-    <row r="946" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A946" s="4"/>
-    </row>
-    <row r="947" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A947" s="4"/>
-    </row>
-    <row r="948" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A948" s="4"/>
-    </row>
-    <row r="949" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A949" s="4"/>
-    </row>
-    <row r="950" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A950" s="4"/>
-    </row>
-    <row r="951" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A951" s="4"/>
+      <c r="A944" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B944" t="s">
+        <v>324</v>
+      </c>
+      <c r="C944" t="s">
+        <v>325</v>
+      </c>
+      <c r="D944" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="945" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A945" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B945" t="s">
+        <v>324</v>
+      </c>
+      <c r="C945" t="s">
+        <v>325</v>
+      </c>
+      <c r="D945" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="946" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A946" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B946" t="s">
+        <v>324</v>
+      </c>
+      <c r="C946" t="s">
+        <v>325</v>
+      </c>
+      <c r="D946" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="947" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A947" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B947" t="s">
+        <v>324</v>
+      </c>
+      <c r="C947" t="s">
+        <v>325</v>
+      </c>
+      <c r="D947" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="948" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A948" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B948" t="s">
+        <v>324</v>
+      </c>
+      <c r="C948" t="s">
+        <v>325</v>
+      </c>
+      <c r="D948" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="949" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A949" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B949" t="s">
+        <v>324</v>
+      </c>
+      <c r="C949" t="s">
+        <v>325</v>
+      </c>
+      <c r="D949" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="950" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A950" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B950" t="s">
+        <v>317</v>
+      </c>
+      <c r="C950" t="s">
+        <v>316</v>
+      </c>
+      <c r="D950" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="951" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A951" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B951" t="s">
+        <v>318</v>
+      </c>
+      <c r="C951" t="s">
+        <v>314</v>
+      </c>
+      <c r="D951" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="952" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A952" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B952" t="s">
+        <v>319</v>
+      </c>
+      <c r="C952" t="s">
+        <v>315</v>
+      </c>
+      <c r="D952" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="953" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A953" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B953" t="s">
+        <v>317</v>
+      </c>
+      <c r="C953" t="s">
+        <v>316</v>
+      </c>
+      <c r="D953" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="954" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A954" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B954" t="s">
+        <v>318</v>
+      </c>
+      <c r="C954" t="s">
+        <v>314</v>
+      </c>
+      <c r="D954" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="955" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A955" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B955" t="s">
+        <v>319</v>
+      </c>
+      <c r="C955" t="s">
+        <v>315</v>
+      </c>
+      <c r="D955" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="956" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A956" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B956" t="s">
+        <v>317</v>
+      </c>
+      <c r="C956" t="s">
+        <v>316</v>
+      </c>
+      <c r="D956" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="957" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A957" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B957" t="s">
+        <v>318</v>
+      </c>
+      <c r="C957" t="s">
+        <v>314</v>
+      </c>
+      <c r="D957" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="958" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A958" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B958" t="s">
+        <v>319</v>
+      </c>
+      <c r="C958" t="s">
+        <v>315</v>
+      </c>
+      <c r="D958" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="959" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A959" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B959" t="s">
+        <v>317</v>
+      </c>
+      <c r="C959" t="s">
+        <v>316</v>
+      </c>
+      <c r="D959" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="960" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A960" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B960" t="s">
+        <v>318</v>
+      </c>
+      <c r="C960" t="s">
+        <v>314</v>
+      </c>
+      <c r="D960" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="961" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A961" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B961" t="s">
+        <v>319</v>
+      </c>
+      <c r="C961" t="s">
+        <v>315</v>
+      </c>
+      <c r="D961" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="962" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A962" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B962" t="s">
+        <v>317</v>
+      </c>
+      <c r="C962" t="s">
+        <v>316</v>
+      </c>
+      <c r="D962" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="963" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A963" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B963" t="s">
+        <v>318</v>
+      </c>
+      <c r="C963" t="s">
+        <v>314</v>
+      </c>
+      <c r="D963" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="964" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A964" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B964" t="s">
+        <v>319</v>
+      </c>
+      <c r="C964" t="s">
+        <v>315</v>
+      </c>
+      <c r="D964" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="965" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A965" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B965" t="s">
+        <v>317</v>
+      </c>
+      <c r="C965" t="s">
+        <v>316</v>
+      </c>
+      <c r="D965" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="966" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A966" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B966" t="s">
+        <v>318</v>
+      </c>
+      <c r="C966" t="s">
+        <v>314</v>
+      </c>
+      <c r="D966" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="967" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A967" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B967" t="s">
+        <v>319</v>
+      </c>
+      <c r="C967" t="s">
+        <v>315</v>
+      </c>
+      <c r="D967" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="968" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A968" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B968" t="s">
+        <v>332</v>
+      </c>
+      <c r="C968" t="s">
+        <v>326</v>
+      </c>
+      <c r="D968" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="969" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A969" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B969" t="s">
+        <v>332</v>
+      </c>
+      <c r="C969" t="s">
+        <v>326</v>
+      </c>
+      <c r="D969" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="970" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A970" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B970" t="s">
+        <v>332</v>
+      </c>
+      <c r="C970" t="s">
+        <v>326</v>
+      </c>
+      <c r="D970" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="971" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A971" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B971" t="s">
+        <v>332</v>
+      </c>
+      <c r="C971" t="s">
+        <v>326</v>
+      </c>
+      <c r="D971" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="972" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A972" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B972" t="s">
+        <v>332</v>
+      </c>
+      <c r="C972" t="s">
+        <v>326</v>
+      </c>
+      <c r="D972" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="973" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A973" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B973" t="s">
+        <v>332</v>
+      </c>
+      <c r="C973" t="s">
+        <v>326</v>
+      </c>
+      <c r="D973" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="974" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A974" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B974" t="s">
+        <v>333</v>
+      </c>
+      <c r="C974" t="s">
+        <v>327</v>
+      </c>
+      <c r="D974" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="975" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A975" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B975" t="s">
+        <v>333</v>
+      </c>
+      <c r="C975" t="s">
+        <v>327</v>
+      </c>
+      <c r="D975" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="976" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A976" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B976" t="s">
+        <v>333</v>
+      </c>
+      <c r="C976" t="s">
+        <v>327</v>
+      </c>
+      <c r="D976" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="977" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A977" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B977" t="s">
+        <v>333</v>
+      </c>
+      <c r="C977" t="s">
+        <v>327</v>
+      </c>
+      <c r="D977" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="978" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A978" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B978" t="s">
+        <v>333</v>
+      </c>
+      <c r="C978" t="s">
+        <v>327</v>
+      </c>
+      <c r="D978" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="979" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A979" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B979" t="s">
+        <v>333</v>
+      </c>
+      <c r="C979" t="s">
+        <v>327</v>
+      </c>
+      <c r="D979" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="980" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A980" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B980" t="s">
+        <v>334</v>
+      </c>
+      <c r="C980" t="s">
+        <v>328</v>
+      </c>
+      <c r="D980" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="981" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A981" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B981" t="s">
+        <v>334</v>
+      </c>
+      <c r="C981" t="s">
+        <v>328</v>
+      </c>
+      <c r="D981" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="982" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A982" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B982" t="s">
+        <v>334</v>
+      </c>
+      <c r="C982" t="s">
+        <v>328</v>
+      </c>
+      <c r="D982" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="983" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A983" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B983" t="s">
+        <v>334</v>
+      </c>
+      <c r="C983" t="s">
+        <v>328</v>
+      </c>
+      <c r="D983" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="984" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A984" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B984" t="s">
+        <v>334</v>
+      </c>
+      <c r="C984" t="s">
+        <v>328</v>
+      </c>
+      <c r="D984" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="985" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A985" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B985" t="s">
+        <v>334</v>
+      </c>
+      <c r="C985" t="s">
+        <v>328</v>
+      </c>
+      <c r="D985" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="986" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A986" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B986" t="s">
+        <v>335</v>
+      </c>
+      <c r="C986" t="s">
+        <v>329</v>
+      </c>
+      <c r="D986" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="987" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A987" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B987" t="s">
+        <v>336</v>
+      </c>
+      <c r="C987" t="s">
+        <v>330</v>
+      </c>
+      <c r="D987" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="988" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A988" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B988" t="s">
+        <v>337</v>
+      </c>
+      <c r="C988" t="s">
+        <v>331</v>
+      </c>
+      <c r="D988" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="989" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A989" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B989" t="s">
+        <v>335</v>
+      </c>
+      <c r="C989" t="s">
+        <v>329</v>
+      </c>
+      <c r="D989" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="990" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A990" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B990" t="s">
+        <v>336</v>
+      </c>
+      <c r="C990" t="s">
+        <v>330</v>
+      </c>
+      <c r="D990" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="991" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A991" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B991" t="s">
+        <v>337</v>
+      </c>
+      <c r="C991" t="s">
+        <v>331</v>
+      </c>
+      <c r="D991" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="992" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A992" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B992" t="s">
+        <v>335</v>
+      </c>
+      <c r="C992" t="s">
+        <v>329</v>
+      </c>
+      <c r="D992" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="993" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A993" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B993" t="s">
+        <v>336</v>
+      </c>
+      <c r="C993" t="s">
+        <v>330</v>
+      </c>
+      <c r="D993" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="994" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A994" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B994" t="s">
+        <v>337</v>
+      </c>
+      <c r="C994" t="s">
+        <v>331</v>
+      </c>
+      <c r="D994" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="995" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A995" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B995" t="s">
+        <v>335</v>
+      </c>
+      <c r="C995" t="s">
+        <v>329</v>
+      </c>
+      <c r="D995" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="996" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A996" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B996" t="s">
+        <v>336</v>
+      </c>
+      <c r="C996" t="s">
+        <v>330</v>
+      </c>
+      <c r="D996" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="997" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A997" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B997" t="s">
+        <v>337</v>
+      </c>
+      <c r="C997" t="s">
+        <v>331</v>
+      </c>
+      <c r="D997" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="998" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A998" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B998" t="s">
+        <v>335</v>
+      </c>
+      <c r="C998" t="s">
+        <v>329</v>
+      </c>
+      <c r="D998" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="999" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A999" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B999" t="s">
+        <v>336</v>
+      </c>
+      <c r="C999" t="s">
+        <v>330</v>
+      </c>
+      <c r="D999" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1000" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1000" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1001" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1001" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1002" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>330</v>
+      </c>
+      <c r="D1002" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1003" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1003" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1004" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1004" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1005" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1005" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1006" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1006" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1007" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1007" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1008" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1008" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1009" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1009" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1010" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1010" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1011" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1011" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1012" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1012" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1013" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1013" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1014" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1014" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1015" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1015" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1016" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1016" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1017" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1017" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1018" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1018" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1019" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1019" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1020" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1020" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1021" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1021" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1022" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1022" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1023" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1023" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1024" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1024" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1025" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1025" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1026" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1026" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1027" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1027" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1028" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1028" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1029" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1029" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1030" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1030" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1031" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1031" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1032" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1032" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1033" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1033" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1034" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1034" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1035" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1035" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1036" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1036" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1037" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1037" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1038" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1038" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1039" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1039" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1040" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1040" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1041" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1041" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1042" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1042" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1043" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1043" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1044" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1044" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1045" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1045" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1046" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1046" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1047" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1047" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1048" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1048" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1049" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1049" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1050" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1050" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1051" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>357</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1051" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1052" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1052" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1053" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1053" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1054" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1054" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1055" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1055" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1056" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1056" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1057" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1057" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1058" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1058" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1059" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1059" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1060" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1060" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1061" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1061" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1062" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1062" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1063" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1063" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1064" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1064" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1065" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1065" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1066" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1066" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1067" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1067" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1068" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1068" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1069" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1069" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1070" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1070" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1071" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1071" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1072" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1072" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1072" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1073" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1073" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1073" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1074" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1074" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1075" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1075" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1076" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1076" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1076" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1077" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1077" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1077" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1078" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1078" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1079" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1079" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1080" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1080" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1080" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1081" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1081" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1081" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1082" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1082" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1083" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1083" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1084" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1084" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1085" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1085" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1086" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1086" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1087" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1087" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1088" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1088" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1089" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1089" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1090" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1090" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1091" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1091" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1092" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1092" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1093" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1093" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1094" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1094" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1095" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1095" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1096" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>367</v>
+      </c>
+      <c r="D1096" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1097" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1097" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1098" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1098" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1099" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>367</v>
+      </c>
+      <c r="D1099" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1100" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1100" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1101" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1101" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1102" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>367</v>
+      </c>
+      <c r="D1102" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1103" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1103" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1104" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1104" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1105" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>367</v>
+      </c>
+      <c r="D1105" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1106" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1106" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1107" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1107" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1108" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>367</v>
+      </c>
+      <c r="D1108" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1109" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1109" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1110" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1110" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1111" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>367</v>
+      </c>
+      <c r="D1111" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1112" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1112" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1113" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1113" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1114" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1114" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1115" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1115" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1116" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1116" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1117" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1117" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1118" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1118" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1119" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1119" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1120" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1120" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1121" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1121" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1122" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1122" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1123" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1123" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1124" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1124" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1125" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1125" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1126" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1126" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1127" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1127" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1128" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1128" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1128" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1129" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1129" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1129" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1130" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1130" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1131" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1131" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1132" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1132" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1132" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1133" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1133" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1133" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1134" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1134" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1134" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1135" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1135" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1136" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1136" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1136" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1137" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1137" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1137" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1138" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1138" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1139" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1139" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1140" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1140" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1140" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1141" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1141" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1141" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1142" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1142" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1143" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1143" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1144" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1144" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1144" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1145" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1145" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1145" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1146" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1146" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1147" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>385</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1147" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1148" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1148" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1148" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1149" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1149" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1149" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1150" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1150" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1151" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1151" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1152" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1152" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1153" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1153" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1154" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1154" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1155" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1155" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1156" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1156" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1157" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1157" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1158" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1158" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1159" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1159" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1160" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1160" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1161" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1161" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1162" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1162" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1163" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1163" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1164" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1164" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1165" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1165" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1166" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1166" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1167" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1167" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1168" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1168" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1169" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1169" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1170" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1170" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1171" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1171" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1172" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1172" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1173" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1173" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1174" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1174" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1175" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1175" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1176" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1176" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1177" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1177" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1178" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1178" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1179" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1179" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1180" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1180" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1180" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1181" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1181" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1181" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1182" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1182" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1182" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1183" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>397</v>
+      </c>
+      <c r="C1183" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1183" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1184" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1184" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1184" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1185" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1185" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1185" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1186" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1186" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1187" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1187" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1188" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1188" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1188" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1189" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1189" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1189" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1190" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1190" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1190" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1191" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1191" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1191" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1192" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1192" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1192" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1193" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1193" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1193" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1194" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1194" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1194" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1195" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>405</v>
+      </c>
+      <c r="C1195" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1195" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1196" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1196" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1196" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1197" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1197" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1197" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1198" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1198" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1198" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1199" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1199" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1199" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1200" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1200" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1200" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1201" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1201" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1201" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1202" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1202" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1202" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1203" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1203" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1203" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1204" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1204" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1204" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1205" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1205" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1205" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1206" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1206" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1206" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1207" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1207" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1207" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1208" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1208" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1208" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1209" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1209" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1209" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1210" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1210" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1210" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1211" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1211" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1211" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1212" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1212" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1212" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1213" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1213" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1213" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1214" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1214" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1214" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1215" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1215" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1215" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1216" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1216" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1216" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1217" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1217" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1217" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1218" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1218" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1218" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1219" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1219" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1219" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1220" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1220" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1220" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
added templates for sms
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78468D9C-5FFE-4353-AB34-76DE9A0DD193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A3A26F-95A9-4C85-8CA3-08DCC114D7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4880" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5456" uniqueCount="460">
   <si>
     <t>lang_code</t>
   </si>
@@ -1264,6 +1264,150 @@
   </si>
   <si>
     <t>acknowledgement-share-cred-with-partner</t>
+  </si>
+  <si>
+    <t>Request received sms to customize and download my card</t>
+  </si>
+  <si>
+    <t>Success sms to customize and download my card</t>
+  </si>
+  <si>
+    <t>Failure sms to customize and download my card</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-request-received_SMS</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-success_SMS</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-failure_SMS</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-request-received_SMS</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-success_SMS</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-failure_SMS</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-request-received_SMS</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-success_SMS</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-failure_SMS</t>
+  </si>
+  <si>
+    <t>update-demo-data-request-received_SMS</t>
+  </si>
+  <si>
+    <t>update-demo-data-success_SMS</t>
+  </si>
+  <si>
+    <t>update-demo-data-failure_SMS</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-request-received_SMS</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-success_SMS</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-failure_SMS</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-request-received_SMS</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-success_SMS</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-failure_SMS</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-request-received_SMS</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-success_SMS</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-failure_SMS</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-request-received_SMS</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-success_SMS</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-failure_SMS</t>
+  </si>
+  <si>
+    <t>Request received sms to order a physical card</t>
+  </si>
+  <si>
+    <t>Success sms to order a physical card</t>
+  </si>
+  <si>
+    <t>Failure sms to order a physical card</t>
+  </si>
+  <si>
+    <t>Request received sms to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Success sms to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Failure sms to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Request received sms to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Success sms to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Failure sms to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Request received sms to self update demographic data</t>
+  </si>
+  <si>
+    <t>Success sms to self update demographic data</t>
+  </si>
+  <si>
+    <t>Failure sms to self update demographic data</t>
+  </si>
+  <si>
+    <t>Request received sms to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Success sms to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Failure sms to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Request received sms to get my UIN card</t>
+  </si>
+  <si>
+    <t>Success sms to get my UIN card</t>
+  </si>
+  <si>
+    <t>Failure sms to get my UIN card</t>
+  </si>
+  <si>
+    <t>Request received sms to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Success sms to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Failure sms to verify my phone and email</t>
   </si>
 </sst>
 </file>
@@ -1638,10 +1782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1220"/>
+  <dimension ref="A1:D1364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1212" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1223" sqref="C1223"/>
+    <sheetView tabSelected="1" topLeftCell="A1355" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1366" sqref="E1366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18731,6 +18875,2022 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1221" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1221" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1221" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1222" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>437</v>
+      </c>
+      <c r="C1222" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1222" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1223" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1223" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1223" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1224" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1224" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1224" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1225" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>437</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1225" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1226" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1226" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1227" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1227" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1228" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>437</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1228" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1229" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1229" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1230" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1230" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1231" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>437</v>
+      </c>
+      <c r="C1231" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1231" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1232" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1232" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1232" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1233" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1233" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1234" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>437</v>
+      </c>
+      <c r="C1234" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1234" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1235" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1235" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1235" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1236" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1236" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1236" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1237" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>437</v>
+      </c>
+      <c r="C1237" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1237" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1238" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1238" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1238" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1239" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1239" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1239" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1240" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1240" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1240" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1241" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1241" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1242" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1242" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1242" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1243" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1243" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1243" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1244" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1244" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1244" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1245" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1245" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1245" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1246" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1246" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1246" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1247" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1247" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1247" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1248" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1248" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1248" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1249" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1249" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1249" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1250" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1250" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1250" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1251" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1251" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1251" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1252" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1252" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1252" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1253" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1253" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1253" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1254" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1254" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1254" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1255" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>416</v>
+      </c>
+      <c r="C1255" t="s">
+        <v>440</v>
+      </c>
+      <c r="D1255" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1256" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1256" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1256" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1257" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1257" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1257" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1258" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1258" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1258" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1259" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1259" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1259" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1260" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1260" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1260" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1261" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1261" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1261" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1262" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1262" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1262" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1263" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1263" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1263" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1264" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1264" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1264" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1265" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1265" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1265" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1266" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1266" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1266" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1267" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1267" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1267" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1268" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1268" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1268" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1269" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1269" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1269" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1270" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1270" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1270" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1271" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1271" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1271" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1272" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1272" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1272" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1273" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1273" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1273" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1274" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1274" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1274" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1275" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1275" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1275" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1276" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1276" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1276" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1277" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1277" t="s">
+        <v>447</v>
+      </c>
+      <c r="D1277" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1278" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1278" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1278" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1279" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1279" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1279" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1280" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1280" t="s">
+        <v>447</v>
+      </c>
+      <c r="D1280" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1281" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1281" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1281" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1282" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1282" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1282" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1283" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1283" t="s">
+        <v>447</v>
+      </c>
+      <c r="D1283" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1284" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1284" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1284" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1285" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1285" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1285" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1286" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1286" t="s">
+        <v>447</v>
+      </c>
+      <c r="D1286" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1287" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1287" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1287" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1288" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1288" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1288" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1288" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1289" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1289" t="s">
+        <v>447</v>
+      </c>
+      <c r="D1289" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1290" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1290" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1290" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1290" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1291" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1291" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1291" t="s">
+        <v>446</v>
+      </c>
+      <c r="D1291" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1292" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1292" t="s">
+        <v>447</v>
+      </c>
+      <c r="D1292" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1293" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1293" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1293" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1294" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>425</v>
+      </c>
+      <c r="C1294" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1294" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1295" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1295" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1295" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1296" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1296" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1296" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1296" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1297" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1297" t="s">
+        <v>425</v>
+      </c>
+      <c r="C1297" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1297" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1298" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1298" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1298" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1298" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1299" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1299" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1299" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1300" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>425</v>
+      </c>
+      <c r="C1300" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1300" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1301" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1301" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1301" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1302" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1302" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1302" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1302" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1303" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1303" t="s">
+        <v>425</v>
+      </c>
+      <c r="C1303" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1303" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1304" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1304" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1304" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1304" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1305" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1305" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1305" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1305" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1306" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1306" t="s">
+        <v>425</v>
+      </c>
+      <c r="C1306" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1306" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1307" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1307" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1307" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1307" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1308" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1308" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1308" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1308" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1309" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1309" t="s">
+        <v>425</v>
+      </c>
+      <c r="C1309" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1309" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1310" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1310" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1310" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1310" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1311" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1311" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1311" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1311" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1312" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1312" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1312" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1313" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1313" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1313" t="s">
+        <v>453</v>
+      </c>
+      <c r="D1313" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1314" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1314" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1314" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1314" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1315" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1315" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1315" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1315" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1316" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1316" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1316" t="s">
+        <v>453</v>
+      </c>
+      <c r="D1316" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1317" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1317" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1317" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1317" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1318" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1318" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1318" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1318" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1319" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1319" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1319" t="s">
+        <v>453</v>
+      </c>
+      <c r="D1319" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1320" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1320" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1320" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1320" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1321" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1321" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1321" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1321" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1322" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1322" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1322" t="s">
+        <v>453</v>
+      </c>
+      <c r="D1322" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1323" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1323" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1323" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1323" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1324" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1324" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1324" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1324" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1325" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1325" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1325" t="s">
+        <v>453</v>
+      </c>
+      <c r="D1325" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1326" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1326" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1326" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1326" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1327" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1327" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1327" t="s">
+        <v>452</v>
+      </c>
+      <c r="D1327" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1328" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1328" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1328" t="s">
+        <v>453</v>
+      </c>
+      <c r="D1328" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1329" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1329" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1329" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1329" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1330" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1330" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1330" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1330" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1331" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1331" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1331" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1331" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1332" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1332" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1332" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1332" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1333" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1333" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1333" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1333" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1334" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1334" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1334" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1334" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1335" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1335" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1335" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1335" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1336" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1336" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1336" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1336" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1337" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1337" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1337" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1337" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1338" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1338" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1338" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1338" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1339" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1339" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1339" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1339" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1340" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1340" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1340" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1340" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1341" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1341" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1341" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1341" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1342" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1342" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1342" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1342" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1343" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1343" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1343" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1343" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1344" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1344" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1344" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1344" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1345" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1345" t="s">
+        <v>431</v>
+      </c>
+      <c r="C1345" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1345" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1346" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1346" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1346" t="s">
+        <v>456</v>
+      </c>
+      <c r="D1346" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1347" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1347" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1347" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1347" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1348" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1348" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1348" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1348" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1349" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1349" t="s">
+        <v>435</v>
+      </c>
+      <c r="C1349" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1349" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1350" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1350" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1350" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1350" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1351" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1351" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1351" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1351" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1352" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1352" t="s">
+        <v>435</v>
+      </c>
+      <c r="C1352" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1352" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1353" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1353" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1353" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1353" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1354" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1354" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1354" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1354" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1355" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1355" t="s">
+        <v>435</v>
+      </c>
+      <c r="C1355" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1355" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1356" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1356" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1356" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1356" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1357" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1357" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1357" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1357" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1358" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1358" t="s">
+        <v>435</v>
+      </c>
+      <c r="C1358" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1358" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1359" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1359" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1359" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1359" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1360" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1360" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1360" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1360" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1361" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1361" t="s">
+        <v>435</v>
+      </c>
+      <c r="C1361" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1361" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1362" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1362" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1362" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1362" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1363" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1363" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1363" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1363" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1364" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1364" t="s">
+        <v>435</v>
+      </c>
+      <c r="C1364" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1364" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
added templates for bell icon notifications
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A3A26F-95A9-4C85-8CA3-08DCC114D7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FF07AF-CA2A-48CC-A45E-007DD100793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5456" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6032" uniqueCount="508">
   <si>
     <t>lang_code</t>
   </si>
@@ -1408,6 +1408,150 @@
   </si>
   <si>
     <t>Failure sms to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Request received bell notify to customize and download my card</t>
+  </si>
+  <si>
+    <t>Success bell notify to customize and download my card</t>
+  </si>
+  <si>
+    <t>Failure bell notify to customize and download my card</t>
+  </si>
+  <si>
+    <t>Request received bell notify to order a physical card</t>
+  </si>
+  <si>
+    <t>Success bell notify to order a physical card</t>
+  </si>
+  <si>
+    <t>Failure bell notify to order a physical card</t>
+  </si>
+  <si>
+    <t>Request received bell notify to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Success bell notify to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Failure bell notify to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Request received bell notify to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Success bell notify to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Failure bell notify to lock/unlock authentication</t>
+  </si>
+  <si>
+    <t>Request received bell notify to self update demographic data</t>
+  </si>
+  <si>
+    <t>Success bell notify to self update demographic data</t>
+  </si>
+  <si>
+    <t>Failure bell notify to self update demographic data</t>
+  </si>
+  <si>
+    <t>Request received bell notify to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Success bell notify to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Failure bell notify to generate or revoke VID</t>
+  </si>
+  <si>
+    <t>Request received bell notify to get my UIN card</t>
+  </si>
+  <si>
+    <t>Success bell notify to get my UIN card</t>
+  </si>
+  <si>
+    <t>Failure bell notify to get my UIN card</t>
+  </si>
+  <si>
+    <t>Request received bell notify to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Success bell notify to verify my phone and email</t>
+  </si>
+  <si>
+    <t>Failure bell notify to verify my phone and email</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-request-received_BELL</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-success_BELL</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-failure_BELL</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-request-received_BELL</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-success_BELL</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-failure_BELL</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-request-received_BELL</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-success_BELL</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-failure_BELL</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-request-received_BELL</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-success_BELL</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-failure_BELL</t>
+  </si>
+  <si>
+    <t>update-demo-data-request-received_BELL</t>
+  </si>
+  <si>
+    <t>update-demo-data-success_BELL</t>
+  </si>
+  <si>
+    <t>update-demo-data-failure_BELL</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-request-received_BELL</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-success_BELL</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-failure_BELL</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-request-received_BELL</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-success_BELL</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-failure_BELL</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-request-received_BELL</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-success_BELL</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-failure_BELL</t>
   </si>
 </sst>
 </file>
@@ -1782,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1364"/>
+  <dimension ref="A1:D1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1355" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1366" sqref="E1366"/>
+    <sheetView tabSelected="1" topLeftCell="A1501" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1374" sqref="C1374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20891,6 +21035,2022 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1365" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1365" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1365" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1365" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1366" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1366" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1366" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1366" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1367" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1367" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1367" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1367" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1368" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1368" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1368" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1368" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1369" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1369" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1369" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1369" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1370" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1370" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1370" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1370" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1371" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1371" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1371" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1371" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1372" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1372" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1372" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1372" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1373" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1373" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1373" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1373" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1374" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1374" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1374" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1374" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1375" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1375" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1375" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1375" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1376" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1376" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1376" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1376" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1377" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1377" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1377" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1377" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1378" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1378" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1378" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1378" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1379" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1379" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1379" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1379" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1380" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1380" t="s">
+        <v>484</v>
+      </c>
+      <c r="C1380" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1380" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1381" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1381" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1381" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1381" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1382" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1382" t="s">
+        <v>486</v>
+      </c>
+      <c r="C1382" t="s">
+        <v>462</v>
+      </c>
+      <c r="D1382" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1383" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1383" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1383" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1383" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1384" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1384" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1384" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1384" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1385" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1385" t="s">
+        <v>489</v>
+      </c>
+      <c r="C1385" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1385" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1386" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1386" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1386" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1387" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1387" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1387" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1387" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1388" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1388" t="s">
+        <v>489</v>
+      </c>
+      <c r="C1388" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1388" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1389" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1389" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1389" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1389" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1390" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1390" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1390" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1390" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1391" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1391" t="s">
+        <v>489</v>
+      </c>
+      <c r="C1391" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1391" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1392" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1392" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1392" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1393" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1393" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1393" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1394" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1394" t="s">
+        <v>489</v>
+      </c>
+      <c r="C1394" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1394" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1395" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1395" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1395" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1396" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1396" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1396" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1397" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1397" t="s">
+        <v>489</v>
+      </c>
+      <c r="C1397" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1397" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1398" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1398" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1398" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1399" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1399" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1399" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1400" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1400" t="s">
+        <v>489</v>
+      </c>
+      <c r="C1400" t="s">
+        <v>465</v>
+      </c>
+      <c r="D1400" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1401" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1401" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1401" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1402" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1402" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1402" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1403" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1403" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1403" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1404" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1404" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1404" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1405" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1405" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1405" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1406" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1406" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1406" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1407" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1407" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1407" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1408" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1408" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1408" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1408" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1409" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1409" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1409" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1409" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1410" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1410" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1410" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1410" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1411" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1411" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1411" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1411" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1412" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1412" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1412" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1412" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1413" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1413" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1413" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1413" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1414" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1414" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1414" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1414" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1415" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1415" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1415" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1415" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1416" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1416" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1416" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1416" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1417" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1417" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1417" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1417" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1418" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1418" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1418" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1418" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1419" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1419" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1419" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1419" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1420" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1420" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1420" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1420" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1421" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1421" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1421" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1421" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1422" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1422" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1422" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1422" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1423" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1423" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1423" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1423" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1424" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1424" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1424" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1424" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1425" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1425" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1425" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1425" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1426" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1426" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1426" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1426" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1427" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1427" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1427" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1427" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1428" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1428" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1428" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1428" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1429" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1429" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1429" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1429" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1430" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1430" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1430" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1430" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1431" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1431" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1431" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1431" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1432" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1432" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1432" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1432" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1433" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1433" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1433" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1433" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1434" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1434" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1434" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1434" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1435" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1435" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1435" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1435" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1436" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1436" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1436" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1436" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1437" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1437" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1437" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1437" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1438" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1438" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1438" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1438" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1439" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1439" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1439" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1439" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1440" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1440" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1440" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1440" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1441" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1441" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1441" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1441" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1442" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1442" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1442" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1442" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1443" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1443" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1443" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1443" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1444" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1444" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1444" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1444" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1445" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1445" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1445" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1445" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1446" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1446" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1446" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1446" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1447" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1447" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1447" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1447" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1448" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1448" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1448" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1448" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1449" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1449" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1449" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1449" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1450" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1450" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1450" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1450" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1451" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1451" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1451" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1451" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1452" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1452" t="s">
+        <v>496</v>
+      </c>
+      <c r="C1452" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1452" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1453" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1453" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1453" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1453" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1454" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1454" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1454" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1454" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1455" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1455" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1455" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1455" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1456" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1456" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1456" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1456" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1457" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1457" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1457" t="s">
+        <v>477</v>
+      </c>
+      <c r="D1457" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1458" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1458" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1458" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1458" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1459" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1459" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1459" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1459" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1460" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1460" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1460" t="s">
+        <v>477</v>
+      </c>
+      <c r="D1460" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1461" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1461" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1461" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1461" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1462" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1462" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1462" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1462" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1463" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1463" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1463" t="s">
+        <v>477</v>
+      </c>
+      <c r="D1463" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1464" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1464" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1464" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1464" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1465" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1465" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1465" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1465" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1466" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1466" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1466" t="s">
+        <v>477</v>
+      </c>
+      <c r="D1466" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1467" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1467" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1467" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1467" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1468" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1468" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1468" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1468" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1469" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1469" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1469" t="s">
+        <v>477</v>
+      </c>
+      <c r="D1469" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1470" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1470" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1470" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1470" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1471" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1471" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1471" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1471" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1472" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1472" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1472" t="s">
+        <v>477</v>
+      </c>
+      <c r="D1472" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1473" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1473" t="s">
+        <v>502</v>
+      </c>
+      <c r="C1473" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1473" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1474" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1474" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1474" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1474" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1475" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1475" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1475" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1475" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1476" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1476" t="s">
+        <v>502</v>
+      </c>
+      <c r="C1476" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1476" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1477" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1477" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1477" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1477" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1478" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1478" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1478" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1478" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1479" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1479" t="s">
+        <v>502</v>
+      </c>
+      <c r="C1479" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1479" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1480" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1480" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1480" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1480" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1481" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1481" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1481" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1481" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1482" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1482" t="s">
+        <v>502</v>
+      </c>
+      <c r="C1482" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1482" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1483" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1483" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1483" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1483" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1484" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1484" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1484" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1484" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1485" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1485" t="s">
+        <v>502</v>
+      </c>
+      <c r="C1485" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1485" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1486" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1486" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1486" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1486" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1487" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1487" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1487" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1487" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1488" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1488" t="s">
+        <v>502</v>
+      </c>
+      <c r="C1488" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1488" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1489" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1489" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1489" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1489" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1490" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1490" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1490" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1490" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1491" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1491" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1491" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1491" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1492" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1492" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1492" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1492" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1493" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1493" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1493" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1493" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1494" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1494" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1494" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1494" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1495" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1495" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1495" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1495" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1496" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1496" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1496" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1496" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1497" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1497" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1497" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1497" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1498" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1498" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1498" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1498" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1499" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1499" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1499" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1499" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1500" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1500" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1500" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1500" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1501" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1501" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1501" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1501" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1502" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1502" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1502" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1502" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1503" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1503" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1503" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1503" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1504" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1504" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1504" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1504" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1505" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1505" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1505" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1505" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1506" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1506" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1506" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1506" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1507" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1507" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1507" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1507" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1508" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1508" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1508" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1508" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
added templates for purpose
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FF07AF-CA2A-48CC-A45E-007DD100793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1066BDBC-FAA1-420C-B08E-022F60BC9692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6032" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6416" uniqueCount="540">
   <si>
     <t>lang_code</t>
   </si>
@@ -1552,6 +1552,102 @@
   </si>
   <si>
     <t>verify-my-phone-email-failure_BELL</t>
+  </si>
+  <si>
+    <t>Positive purpose to customize and download my card</t>
+  </si>
+  <si>
+    <t>Negative purpose to customize and download my card</t>
+  </si>
+  <si>
+    <t>Positive purpose to order a physical card</t>
+  </si>
+  <si>
+    <t>Negative purpose to order a physical card</t>
+  </si>
+  <si>
+    <t>Positive purpose to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Negative purpose to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Positive purpose to lock/unlock various authentication types</t>
+  </si>
+  <si>
+    <t>Negative purpose to lock/unlock various authentication types</t>
+  </si>
+  <si>
+    <t>Positive Purpose to self update demographic data</t>
+  </si>
+  <si>
+    <t>Negative Purpose to self update demographic data</t>
+  </si>
+  <si>
+    <t>Positive Purpose  to generate or revoke VIDs</t>
+  </si>
+  <si>
+    <t>Negative Purpose to generate or revoke VIDs</t>
+  </si>
+  <si>
+    <t>Positive purpose to get my UIN card</t>
+  </si>
+  <si>
+    <t>Negative purpose to get my UIN card</t>
+  </si>
+  <si>
+    <t>Positive purpose to verify my phone number and email ID</t>
+  </si>
+  <si>
+    <t>Negative purpose to verify my phone number and email ID</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-positive-purpose</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-negative-purpose</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-positive purpose</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-negative purpose</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-positive-purpose</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-negative-purpose</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-positive-purpose</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-negative-purpose</t>
+  </si>
+  <si>
+    <t>update-demo-data-positive-purpose</t>
+  </si>
+  <si>
+    <t>update-demo-data-negative-purpose</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-positive-purpose</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-negative-purpose</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-positive-purpose</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-negative-purpose</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-positive-purpose</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-negative-purpose</t>
   </si>
 </sst>
 </file>
@@ -1926,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1508"/>
+  <dimension ref="A1:D1604"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1501" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1374" sqref="C1374"/>
+    <sheetView tabSelected="1" topLeftCell="A1597" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1606" sqref="F1606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23051,6 +23147,1350 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1509" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1509" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1509" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1509" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1509" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1510" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1510" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1510" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1510" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1511" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1511" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1511" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1511" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1512" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1512" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1512" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1512" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1513" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1513" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1513" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1513" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1514" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1514" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1514" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1514" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1515" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1515" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1515" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1515" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1516" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1516" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1516" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1516" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1517" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1517" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1517" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1517" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1518" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1518" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1518" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1518" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1519" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1519" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1519" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1519" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1520" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1520" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1520" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1520" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1521" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1521" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1521" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1521" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1522" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1522" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1522" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1522" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1523" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1523" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1523" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1523" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1524" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1524" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1524" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1524" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1525" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1525" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1525" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1525" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1526" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1526" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1526" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1526" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1527" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1527" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1527" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1527" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1528" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1528" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1528" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1528" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1529" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1529" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1529" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1529" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1530" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1530" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1530" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1530" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1531" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1531" t="s">
+        <v>526</v>
+      </c>
+      <c r="C1531" t="s">
+        <v>510</v>
+      </c>
+      <c r="D1531" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1532" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1532" t="s">
+        <v>527</v>
+      </c>
+      <c r="C1532" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1532" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1533" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1533" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1533" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1533" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1534" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1534" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1534" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1534" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1535" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1535" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1535" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1535" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1536" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1536" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1536" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1536" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1537" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1537" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1537" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1537" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1538" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1538" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1538" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1538" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1539" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1539" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1539" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1539" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1540" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1540" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1540" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1540" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1541" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1541" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1541" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1541" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1542" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1542" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1542" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1542" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1543" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1543" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1543" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1543" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1544" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1544" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1544" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1544" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1545" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1545" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1545" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1545" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1546" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1546" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1546" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1546" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1547" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1547" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1547" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1547" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1548" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1548" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1548" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1548" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1549" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1549" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1549" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1549" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1550" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1550" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1550" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1550" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1551" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1551" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1551" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1551" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1552" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1552" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1552" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1552" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1553" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1553" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1553" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1553" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1554" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1554" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1554" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1554" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1555" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1555" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1555" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1555" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1556" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1556" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1556" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1556" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1557" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1557" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1557" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1557" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1558" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1558" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1558" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1558" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1559" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1559" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1559" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1559" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1560" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1560" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1560" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1560" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1561" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1561" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1561" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1561" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1562" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1562" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1562" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1562" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1563" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1563" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1563" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1563" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1564" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1564" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1564" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1564" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1565" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1565" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1565" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1565" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1566" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1566" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1566" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1566" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1567" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1567" t="s">
+        <v>532</v>
+      </c>
+      <c r="C1567" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1567" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1568" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1568" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1568" t="s">
+        <v>517</v>
+      </c>
+      <c r="D1568" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1569" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1569" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1569" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1569" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1570" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1570" t="s">
+        <v>535</v>
+      </c>
+      <c r="C1570" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1570" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1571" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1571" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1571" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1571" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1572" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1572" t="s">
+        <v>535</v>
+      </c>
+      <c r="C1572" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1572" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1573" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1573" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1573" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1573" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1574" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1574" t="s">
+        <v>535</v>
+      </c>
+      <c r="C1574" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1574" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1575" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1575" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1575" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1575" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1576" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1576" t="s">
+        <v>535</v>
+      </c>
+      <c r="C1576" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1576" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1577" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1577" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1577" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1577" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1578" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1578" t="s">
+        <v>535</v>
+      </c>
+      <c r="C1578" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1578" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1579" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1579" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1579" t="s">
+        <v>518</v>
+      </c>
+      <c r="D1579" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1580" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1580" t="s">
+        <v>535</v>
+      </c>
+      <c r="C1580" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1580" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1581" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1581" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1581" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1581" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1582" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1582" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1582" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1582" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1583" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1583" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1583" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1583" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1584" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1584" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1584" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1584" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1585" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1585" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1585" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1585" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1586" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1586" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1586" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1586" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1587" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1587" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1587" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1587" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1588" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1588" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1588" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1588" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1589" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1589" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1589" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1589" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1590" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1590" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1590" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1590" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1591" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1591" t="s">
+        <v>536</v>
+      </c>
+      <c r="C1591" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1591" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1592" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1592" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1592" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1592" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1593" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1593" t="s">
+        <v>538</v>
+      </c>
+      <c r="C1593" t="s">
+        <v>522</v>
+      </c>
+      <c r="D1593" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1594" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1594" t="s">
+        <v>539</v>
+      </c>
+      <c r="C1594" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1594" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1595" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1595" t="s">
+        <v>538</v>
+      </c>
+      <c r="C1595" t="s">
+        <v>522</v>
+      </c>
+      <c r="D1595" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1596" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1596" t="s">
+        <v>539</v>
+      </c>
+      <c r="C1596" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1596" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1597" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1597" t="s">
+        <v>538</v>
+      </c>
+      <c r="C1597" t="s">
+        <v>522</v>
+      </c>
+      <c r="D1597" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1598" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1598" t="s">
+        <v>539</v>
+      </c>
+      <c r="C1598" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1598" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1599" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1599" t="s">
+        <v>538</v>
+      </c>
+      <c r="C1599" t="s">
+        <v>522</v>
+      </c>
+      <c r="D1599" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1600" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1600" t="s">
+        <v>539</v>
+      </c>
+      <c r="C1600" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1600" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1601" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1601" t="s">
+        <v>538</v>
+      </c>
+      <c r="C1601" t="s">
+        <v>522</v>
+      </c>
+      <c r="D1601" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1602" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1602" t="s">
+        <v>539</v>
+      </c>
+      <c r="C1602" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1602" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1603" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1603" t="s">
+        <v>538</v>
+      </c>
+      <c r="C1603" t="s">
+        <v>522</v>
+      </c>
+      <c r="D1603" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1604" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1604" t="s">
+        <v>539</v>
+      </c>
+      <c r="C1604" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1604" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-23692 Added template for ack in resident service.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D43C53-239F-469D-AB6A-5090435615F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0A10FB-946C-47A9-8512-2F6BEBDA594A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$400</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6616" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6636" uniqueCount="570">
   <si>
     <t>lang_code</t>
   </si>
@@ -1708,13 +1708,43 @@
   </si>
   <si>
     <t>Acknowledgement for manage my vid</t>
+  </si>
+  <si>
+    <t>acknowledgement-order-a-physical-card</t>
+  </si>
+  <si>
+    <t>Acknowledgement for Order a physical card</t>
+  </si>
+  <si>
+    <t>Acknowledgement for Download a personalized card</t>
+  </si>
+  <si>
+    <t>acknowledgement-download-a-personalized-card</t>
+  </si>
+  <si>
+    <t>Acknowledgement for Update demographic data</t>
+  </si>
+  <si>
+    <t>acknowledgement-update-demographic-data</t>
+  </si>
+  <si>
+    <t>acknowledgement-verify-email-id-or-phone-number</t>
+  </si>
+  <si>
+    <t>Acknowledgement for verify email id or phone number</t>
+  </si>
+  <si>
+    <t>acknowledgement-secure-my-id</t>
+  </si>
+  <si>
+    <t>Acknowledgement for Secure my Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1726,7 +1756,13 @@
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1764,7 +1800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1774,6 +1810,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2082,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1654"/>
+  <dimension ref="A1:D1659"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1644" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1655" sqref="A1655"/>
+    <sheetView tabSelected="1" topLeftCell="A1647" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1661" sqref="B1661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25251,9 +25288,79 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1655" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1655" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1655" t="s">
+        <v>560</v>
+      </c>
+      <c r="C1655" t="s">
+        <v>561</v>
+      </c>
+      <c r="D1655" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1656" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1656" t="s">
+        <v>563</v>
+      </c>
+      <c r="C1656" t="s">
+        <v>562</v>
+      </c>
+      <c r="D1656" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1657" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1657" t="s">
+        <v>565</v>
+      </c>
+      <c r="C1657" t="s">
+        <v>564</v>
+      </c>
+      <c r="D1657" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1658" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1658" t="s">
+        <v>566</v>
+      </c>
+      <c r="C1658" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="D1658" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1659" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1659" t="s">
+        <v>568</v>
+      </c>
+      <c r="C1659" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="D1659" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MOSIP-22865 Added template for service history table view.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C090E02-8AFB-4EA5-A652-4A961BC0AD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC9C33A-D6A8-4941-BA27-C383DE8090EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1782,10 +1782,10 @@
     <t>Validate OTP</t>
   </si>
   <si>
-    <t>ack-view-service-history</t>
-  </si>
-  <si>
     <t>Acknowledment view service history</t>
+  </si>
+  <si>
+    <t>service-history-type</t>
   </si>
 </sst>
 </file>
@@ -2169,7 +2169,7 @@
   <dimension ref="A1:D1697"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1688" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1698" sqref="C1698"/>
+      <selection activeCell="A1698" sqref="A1698"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25928,10 +25928,10 @@
         <v>4</v>
       </c>
       <c r="B1697" t="s">
+        <v>585</v>
+      </c>
+      <c r="C1697" t="s">
         <v>584</v>
-      </c>
-      <c r="C1697" t="s">
-        <v>585</v>
       </c>
       <c r="D1697" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
MOSIP-24372 Added template ack for vid card download summary in resident service.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD9B09C-C2D1-4DD9-AA83-8FABE75F73D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D64B20-CC5D-4365-88B7-7DAF28EC80EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6800" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6812" uniqueCount="598">
   <si>
     <t>lang_code</t>
   </si>
@@ -1804,6 +1804,24 @@
   </si>
   <si>
     <t>Acknowledment Get My Id</t>
+  </si>
+  <si>
+    <t>vid-card-download-positive-purpose</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-purpose</t>
+  </si>
+  <si>
+    <t>vid-card-download-positive-summary</t>
+  </si>
+  <si>
+    <t>Vid Card Download Positive Purpose</t>
+  </si>
+  <si>
+    <t>Vid Card Download Failure Purpose</t>
+  </si>
+  <si>
+    <t>Vid Card Download Positive Summary</t>
   </si>
 </sst>
 </file>
@@ -2193,10 +2211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1700"/>
+  <dimension ref="A1:D1703"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1688" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1702" sqref="B1702"/>
+      <selection activeCell="B1703" sqref="B1703"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -26006,6 +26024,48 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1701" spans="1:4">
+      <c r="A1701" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1701" t="s">
+        <v>592</v>
+      </c>
+      <c r="C1701" t="s">
+        <v>595</v>
+      </c>
+      <c r="D1701" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:4">
+      <c r="A1702" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1702" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1702" t="s">
+        <v>596</v>
+      </c>
+      <c r="D1702" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:4">
+      <c r="A1703" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1703" t="s">
+        <v>594</v>
+      </c>
+      <c r="C1703" t="s">
+        <v>597</v>
+      </c>
+      <c r="D1703" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-25864 Corrected template for resident service.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ABF47C-ED22-434A-9978-DA641204EF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337574ED-1CFC-4A0F-8051-07E976BC82F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6812" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6860" uniqueCount="622">
   <si>
     <t>lang_code</t>
   </si>
@@ -1822,13 +1822,85 @@
   </si>
   <si>
     <t>vid-card-download-negative-purpose</t>
+  </si>
+  <si>
+    <t>mosip.idp.otp.template.property</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>mosip.idp.biometrics.template.property</t>
+  </si>
+  <si>
+    <t>Biometrics</t>
+  </si>
+  <si>
+    <t>mosip.idp.unknown.authentication.template.property</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>mosip.full.name.template.property</t>
+  </si>
+  <si>
+    <t>mosip.date.of.birth.template.property</t>
+  </si>
+  <si>
+    <t>mosip.uin.template.property</t>
+  </si>
+  <si>
+    <t>mosip.perpetual.vid.template.property</t>
+  </si>
+  <si>
+    <t>mosip.phone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.email.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.template.property</t>
+  </si>
+  <si>
+    <t>mosip.gender.template.property</t>
+  </si>
+  <si>
+    <t>mosip.defualt.template.property</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>UIN</t>
+  </si>
+  <si>
+    <t>Perpetual VID</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Defualt</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1851,6 +1923,12 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -1890,7 +1968,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1901,6 +1979,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2211,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1703"/>
+  <dimension ref="A1:D1715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1688" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1703" sqref="B1703"/>
+    <sheetView tabSelected="1" topLeftCell="A1700" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1716" sqref="C1716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -26066,6 +26147,174 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1704" spans="1:4">
+      <c r="A1704" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1704" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>599</v>
+      </c>
+      <c r="D1704" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:4">
+      <c r="A1705" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1705" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>601</v>
+      </c>
+      <c r="D1705" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:4">
+      <c r="A1706" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1706" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>603</v>
+      </c>
+      <c r="D1706" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:4">
+      <c r="A1707" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>613</v>
+      </c>
+      <c r="D1707" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:4">
+      <c r="A1708" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>605</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1708" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:4">
+      <c r="A1709" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1709" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:4">
+      <c r="A1710" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1710" t="s">
+        <v>616</v>
+      </c>
+      <c r="D1710" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:4">
+      <c r="A1711" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1711" t="s">
+        <v>617</v>
+      </c>
+      <c r="D1711" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:4">
+      <c r="A1712" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1712" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1712" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:4">
+      <c r="A1713" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>610</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>618</v>
+      </c>
+      <c r="D1713" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:4">
+      <c r="A1714" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1714" t="s">
+        <v>619</v>
+      </c>
+      <c r="D1714" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:4">
+      <c r="A1715" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1715" t="s">
+        <v>620</v>
+      </c>
+      <c r="D1715" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-24773 Added vid card template.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337574ED-1CFC-4A0F-8051-07E976BC82F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835B11E7-AB0A-4B9E-A2E3-D002FA2F9120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6860" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6864" uniqueCount="624">
   <si>
     <t>lang_code</t>
   </si>
@@ -1894,6 +1894,12 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>vid-card-type</t>
+  </si>
+  <si>
+    <t>Vid Card Type</t>
   </si>
 </sst>
 </file>
@@ -2292,10 +2298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1715"/>
+  <dimension ref="A1:D1716"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1700" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1716" sqref="C1716"/>
+    <sheetView tabSelected="1" topLeftCell="A1706" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1716" sqref="B1716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -26315,6 +26321,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1716" spans="1:4">
+      <c r="A1716" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1716" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-26515 Added resident template.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835B11E7-AB0A-4B9E-A2E3-D002FA2F9120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0B56CD-AB7B-4BD9-A295-CFCA527DC959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6864" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6900" uniqueCount="642">
   <si>
     <t>lang_code</t>
   </si>
@@ -1900,6 +1900,60 @@
   </si>
   <si>
     <t>Vid Card Type</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>Request received email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-subject</t>
+  </si>
+  <si>
+    <t>Success email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-subject</t>
+  </si>
+  <si>
+    <t>Failure email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-content</t>
+  </si>
+  <si>
+    <t>Request received email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-content</t>
+  </si>
+  <si>
+    <t>Success email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-content</t>
+  </si>
+  <si>
+    <t>Failure email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received_SMS</t>
+  </si>
+  <si>
+    <t>Request received sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success_SMS</t>
+  </si>
+  <si>
+    <t>Success sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure_SMS</t>
+  </si>
+  <si>
+    <t>Failure sms to download my VID card</t>
   </si>
 </sst>
 </file>
@@ -2298,17 +2352,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1716"/>
+  <dimension ref="A1:D1725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1706" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1716" sqref="B1716"/>
+    <sheetView tabSelected="1" topLeftCell="A1712" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1716" sqref="C1716"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -26332,6 +26386,132 @@
         <v>623</v>
       </c>
       <c r="D1716" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:4">
+      <c r="A1717" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1717" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:4">
+      <c r="A1718" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1718" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:4">
+      <c r="A1719" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>628</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1719" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:4">
+      <c r="A1720" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>630</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1720" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:4">
+      <c r="A1721" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>632</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>633</v>
+      </c>
+      <c r="D1721" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:4">
+      <c r="A1722" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>634</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>635</v>
+      </c>
+      <c r="D1722" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:4">
+      <c r="A1723" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>636</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>637</v>
+      </c>
+      <c r="D1723" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:4">
+      <c r="A1724" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>638</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>639</v>
+      </c>
+      <c r="D1724" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:4">
+      <c r="A1725" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>640</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>641</v>
+      </c>
+      <c r="D1725" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MOSIP-17570 added supervisor rejected email and sms templates (#218)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0B56CD-AB7B-4BD9-A295-CFCA527DC959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6900" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="648">
   <si>
     <t>lang_code</t>
   </si>
@@ -1954,12 +1953,30 @@
   </si>
   <si>
     <t>Failure sms to download my VID card</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_SMS</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject SMS</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -2073,7 +2090,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2351,11 +2368,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1725"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1712" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1716" sqref="C1716"/>
+    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1730" sqref="F1730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26515,8 +26532,260 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1726" spans="1:4">
+      <c r="A1726" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1726" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:4">
+      <c r="A1727" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1727" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:4">
+      <c r="A1728" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1728" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4">
+      <c r="A1729" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1729" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4">
+      <c r="A1730" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1730" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4">
+      <c r="A1731" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1731" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4">
+      <c r="A1732" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1732" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4">
+      <c r="A1733" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1733" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4">
+      <c r="A1734" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1734" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:4">
+      <c r="A1735" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1735" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:4">
+      <c r="A1736" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1736" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:4">
+      <c r="A1737" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1737" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:4">
+      <c r="A1738" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1738" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:4">
+      <c r="A1739" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1739" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:4">
+      <c r="A1740" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1740" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:4">
+      <c r="A1741" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1741" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:4">
+      <c r="A1742" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1742" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:4">
+      <c r="A1743" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1743" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D400"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
MOSIP-26844 Corrected template for resident service. (#226)
* MOSIP-25463 Update view history template for resident service.

* MOSIP-26927 Corrected copyright year for resident template.

* Corrected template for view history.

* Corrected template for resident service.

* Corrected template for resident service.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87778D35-F03C-4626-B422-D54C36170F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$400</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6992" uniqueCount="658">
   <si>
     <t>lang_code</t>
   </si>
@@ -1971,12 +1972,42 @@
   </si>
   <si>
     <t>Template for Supervisor Reject Email Subject</t>
+  </si>
+  <si>
+    <t>mosip.province.template.property</t>
+  </si>
+  <si>
+    <t>mosip.city.template.property</t>
+  </si>
+  <si>
+    <t>mosip.zone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.postal.code.template.property</t>
+  </si>
+  <si>
+    <t>mosip.region.template.property</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -2090,7 +2121,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2368,11 +2399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1743"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1748"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1730" sqref="F1730"/>
+    <sheetView tabSelected="1" topLeftCell="A1705" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1718" sqref="C1718"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26369,10 +26400,10 @@
         <v>4</v>
       </c>
       <c r="B1714" t="s">
-        <v>611</v>
+        <v>648</v>
       </c>
       <c r="C1714" t="s">
-        <v>619</v>
+        <v>653</v>
       </c>
       <c r="D1714" s="1" t="s">
         <v>7</v>
@@ -26383,10 +26414,10 @@
         <v>4</v>
       </c>
       <c r="B1715" t="s">
-        <v>612</v>
+        <v>649</v>
       </c>
       <c r="C1715" t="s">
-        <v>620</v>
+        <v>654</v>
       </c>
       <c r="D1715" s="1" t="s">
         <v>7</v>
@@ -26397,10 +26428,10 @@
         <v>4</v>
       </c>
       <c r="B1716" t="s">
-        <v>622</v>
+        <v>650</v>
       </c>
       <c r="C1716" t="s">
-        <v>623</v>
+        <v>655</v>
       </c>
       <c r="D1716" s="1" t="s">
         <v>7</v>
@@ -26411,10 +26442,10 @@
         <v>4</v>
       </c>
       <c r="B1717" t="s">
-        <v>624</v>
+        <v>651</v>
       </c>
       <c r="C1717" t="s">
-        <v>625</v>
+        <v>657</v>
       </c>
       <c r="D1717" s="1" t="s">
         <v>7</v>
@@ -26425,10 +26456,10 @@
         <v>4</v>
       </c>
       <c r="B1718" t="s">
-        <v>626</v>
+        <v>652</v>
       </c>
       <c r="C1718" t="s">
-        <v>627</v>
+        <v>656</v>
       </c>
       <c r="D1718" s="1" t="s">
         <v>7</v>
@@ -26439,10 +26470,10 @@
         <v>4</v>
       </c>
       <c r="B1719" t="s">
-        <v>628</v>
+        <v>611</v>
       </c>
       <c r="C1719" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="D1719" s="1" t="s">
         <v>7</v>
@@ -26453,10 +26484,10 @@
         <v>4</v>
       </c>
       <c r="B1720" t="s">
-        <v>630</v>
+        <v>612</v>
       </c>
       <c r="C1720" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
       <c r="D1720" s="1" t="s">
         <v>7</v>
@@ -26467,10 +26498,10 @@
         <v>4</v>
       </c>
       <c r="B1721" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="C1721" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="D1721" s="1" t="s">
         <v>7</v>
@@ -26481,10 +26512,10 @@
         <v>4</v>
       </c>
       <c r="B1722" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="C1722" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="D1722" s="1" t="s">
         <v>7</v>
@@ -26495,10 +26526,10 @@
         <v>4</v>
       </c>
       <c r="B1723" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="C1723" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
       <c r="D1723" s="1" t="s">
         <v>7</v>
@@ -26509,10 +26540,10 @@
         <v>4</v>
       </c>
       <c r="B1724" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="C1724" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="D1724" s="1" t="s">
         <v>7</v>
@@ -26523,10 +26554,10 @@
         <v>4</v>
       </c>
       <c r="B1725" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C1725" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="D1725" s="1" t="s">
         <v>7</v>
@@ -26537,10 +26568,10 @@
         <v>4</v>
       </c>
       <c r="B1726" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="C1726" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="D1726" s="1" t="s">
         <v>7</v>
@@ -26551,10 +26582,10 @@
         <v>4</v>
       </c>
       <c r="B1727" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="C1727" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="D1727" s="1" t="s">
         <v>7</v>
@@ -26562,13 +26593,13 @@
     </row>
     <row r="1728" spans="1:4">
       <c r="A1728" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1728" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="C1728" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="D1728" s="1" t="s">
         <v>7</v>
@@ -26576,13 +26607,13 @@
     </row>
     <row r="1729" spans="1:4">
       <c r="A1729" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1729" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="C1729" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="D1729" s="1" t="s">
         <v>7</v>
@@ -26590,13 +26621,13 @@
     </row>
     <row r="1730" spans="1:4">
       <c r="A1730" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B1730" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C1730" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D1730" s="1" t="s">
         <v>7</v>
@@ -26604,13 +26635,13 @@
     </row>
     <row r="1731" spans="1:4">
       <c r="A1731" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B1731" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1731" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1731" s="1" t="s">
         <v>7</v>
@@ -26618,13 +26649,13 @@
     </row>
     <row r="1732" spans="1:4">
       <c r="A1732" t="s">
-        <v>302</v>
+        <v>4</v>
       </c>
       <c r="B1732" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1732" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1732" s="1" t="s">
         <v>7</v>
@@ -26632,13 +26663,13 @@
     </row>
     <row r="1733" spans="1:4">
       <c r="A1733" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B1733" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1733" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1733" s="1" t="s">
         <v>7</v>
@@ -26646,13 +26677,13 @@
     </row>
     <row r="1734" spans="1:4">
       <c r="A1734" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B1734" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1734" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1734" s="1" t="s">
         <v>7</v>
@@ -26660,13 +26691,13 @@
     </row>
     <row r="1735" spans="1:4">
       <c r="A1735" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B1735" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1735" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1735" s="1" t="s">
         <v>7</v>
@@ -26674,13 +26705,13 @@
     </row>
     <row r="1736" spans="1:4">
       <c r="A1736" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B1736" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1736" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1736" s="1" t="s">
         <v>7</v>
@@ -26688,13 +26719,13 @@
     </row>
     <row r="1737" spans="1:4">
       <c r="A1737" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B1737" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1737" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1737" s="1" t="s">
         <v>7</v>
@@ -26702,13 +26733,13 @@
     </row>
     <row r="1738" spans="1:4">
       <c r="A1738" t="s">
-        <v>4</v>
+        <v>302</v>
       </c>
       <c r="B1738" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1738" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1738" s="1" t="s">
         <v>7</v>
@@ -26716,13 +26747,13 @@
     </row>
     <row r="1739" spans="1:4">
       <c r="A1739" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B1739" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C1739" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D1739" s="1" t="s">
         <v>7</v>
@@ -26730,13 +26761,13 @@
     </row>
     <row r="1740" spans="1:4">
       <c r="A1740" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B1740" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1740" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1740" s="1" t="s">
         <v>7</v>
@@ -26744,13 +26775,13 @@
     </row>
     <row r="1741" spans="1:4">
       <c r="A1741" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B1741" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C1741" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D1741" s="1" t="s">
         <v>7</v>
@@ -26758,13 +26789,13 @@
     </row>
     <row r="1742" spans="1:4">
       <c r="A1742" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B1742" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1742" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1742" s="1" t="s">
         <v>7</v>
@@ -26772,7 +26803,7 @@
     </row>
     <row r="1743" spans="1:4">
       <c r="A1743" t="s">
-        <v>303</v>
+        <v>4</v>
       </c>
       <c r="B1743" t="s">
         <v>646</v>
@@ -26784,8 +26815,78 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1744" spans="1:4">
+      <c r="A1744" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1744" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1744" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:4">
+      <c r="A1745" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1745" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1745" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:4">
+      <c r="A1746" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1746" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1746" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:4">
+      <c r="A1747" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1747" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1747" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1747" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:4">
+      <c r="A1748" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1748" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1748" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400"/>
+  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Mosip 26981 resident UI in share my data after download the pdf selected attributes is not showing in the downloaded pdf (#227)
* MOSIP-25463 Update view history template for resident service.

* MOSIP-26927 Corrected copyright year for resident template.

* Corrected template for view history.

* Corrected template for resident service.

* Corrected template for resident service.

* MOSIP-26981-resident-ui-in-share-my-data-after-download-the-pdf-selected-attributes-is-not-showing-in-the-downloaded-pdf
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87778D35-F03C-4626-B422-D54C36170F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1F5D6F-AEEF-4B2A-A358-D97623743B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6992" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7000" uniqueCount="662">
   <si>
     <t>lang_code</t>
   </si>
@@ -2002,6 +2002,18 @@
   </si>
   <si>
     <t>Postal Code</t>
+  </si>
+  <si>
+    <t>mosip.preferred.language.template.property</t>
+  </si>
+  <si>
+    <t>Preferred language</t>
+  </si>
+  <si>
+    <t>mosip.photo.template.property</t>
+  </si>
+  <si>
+    <t>Photo</t>
   </si>
 </sst>
 </file>
@@ -2400,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1748"/>
+  <dimension ref="A1:D1750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1705" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1718" sqref="C1718"/>
+    <sheetView tabSelected="1" topLeftCell="A1716" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1720" sqref="C1720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26484,10 +26496,10 @@
         <v>4</v>
       </c>
       <c r="B1720" t="s">
-        <v>612</v>
+        <v>660</v>
       </c>
       <c r="C1720" t="s">
-        <v>620</v>
+        <v>661</v>
       </c>
       <c r="D1720" s="1" t="s">
         <v>7</v>
@@ -26498,10 +26510,10 @@
         <v>4</v>
       </c>
       <c r="B1721" t="s">
-        <v>622</v>
+        <v>658</v>
       </c>
       <c r="C1721" t="s">
-        <v>623</v>
+        <v>659</v>
       </c>
       <c r="D1721" s="1" t="s">
         <v>7</v>
@@ -26512,10 +26524,10 @@
         <v>4</v>
       </c>
       <c r="B1722" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
       <c r="C1722" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="D1722" s="1" t="s">
         <v>7</v>
@@ -26526,10 +26538,10 @@
         <v>4</v>
       </c>
       <c r="B1723" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C1723" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D1723" s="1" t="s">
         <v>7</v>
@@ -26540,10 +26552,10 @@
         <v>4</v>
       </c>
       <c r="B1724" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C1724" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D1724" s="1" t="s">
         <v>7</v>
@@ -26554,10 +26566,10 @@
         <v>4</v>
       </c>
       <c r="B1725" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C1725" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="D1725" s="1" t="s">
         <v>7</v>
@@ -26568,10 +26580,10 @@
         <v>4</v>
       </c>
       <c r="B1726" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C1726" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="D1726" s="1" t="s">
         <v>7</v>
@@ -26582,10 +26594,10 @@
         <v>4</v>
       </c>
       <c r="B1727" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C1727" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D1727" s="1" t="s">
         <v>7</v>
@@ -26596,10 +26608,10 @@
         <v>4</v>
       </c>
       <c r="B1728" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C1728" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D1728" s="1" t="s">
         <v>7</v>
@@ -26610,10 +26622,10 @@
         <v>4</v>
       </c>
       <c r="B1729" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C1729" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D1729" s="1" t="s">
         <v>7</v>
@@ -26624,10 +26636,10 @@
         <v>4</v>
       </c>
       <c r="B1730" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C1730" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="D1730" s="1" t="s">
         <v>7</v>
@@ -26638,10 +26650,10 @@
         <v>4</v>
       </c>
       <c r="B1731" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C1731" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D1731" s="1" t="s">
         <v>7</v>
@@ -26652,10 +26664,10 @@
         <v>4</v>
       </c>
       <c r="B1732" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C1732" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D1732" s="1" t="s">
         <v>7</v>
@@ -26663,7 +26675,7 @@
     </row>
     <row r="1733" spans="1:4">
       <c r="A1733" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1733" t="s">
         <v>642</v>
@@ -26677,7 +26689,7 @@
     </row>
     <row r="1734" spans="1:4">
       <c r="A1734" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1734" t="s">
         <v>644</v>
@@ -26691,7 +26703,7 @@
     </row>
     <row r="1735" spans="1:4">
       <c r="A1735" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B1735" t="s">
         <v>642</v>
@@ -26705,7 +26717,7 @@
     </row>
     <row r="1736" spans="1:4">
       <c r="A1736" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B1736" t="s">
         <v>644</v>
@@ -26719,7 +26731,7 @@
     </row>
     <row r="1737" spans="1:4">
       <c r="A1737" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B1737" t="s">
         <v>642</v>
@@ -26733,7 +26745,7 @@
     </row>
     <row r="1738" spans="1:4">
       <c r="A1738" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B1738" t="s">
         <v>644</v>
@@ -26747,7 +26759,7 @@
     </row>
     <row r="1739" spans="1:4">
       <c r="A1739" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B1739" t="s">
         <v>642</v>
@@ -26761,7 +26773,7 @@
     </row>
     <row r="1740" spans="1:4">
       <c r="A1740" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B1740" t="s">
         <v>644</v>
@@ -26775,7 +26787,7 @@
     </row>
     <row r="1741" spans="1:4">
       <c r="A1741" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1741" t="s">
         <v>642</v>
@@ -26789,7 +26801,7 @@
     </row>
     <row r="1742" spans="1:4">
       <c r="A1742" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1742" t="s">
         <v>644</v>
@@ -26803,13 +26815,13 @@
     </row>
     <row r="1743" spans="1:4">
       <c r="A1743" t="s">
-        <v>4</v>
+        <v>303</v>
       </c>
       <c r="B1743" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C1743" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D1743" s="1" t="s">
         <v>7</v>
@@ -26817,13 +26829,13 @@
     </row>
     <row r="1744" spans="1:4">
       <c r="A1744" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B1744" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1744" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1744" s="1" t="s">
         <v>7</v>
@@ -26831,7 +26843,7 @@
     </row>
     <row r="1745" spans="1:4">
       <c r="A1745" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B1745" t="s">
         <v>646</v>
@@ -26845,7 +26857,7 @@
     </row>
     <row r="1746" spans="1:4">
       <c r="A1746" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B1746" t="s">
         <v>646</v>
@@ -26859,7 +26871,7 @@
     </row>
     <row r="1747" spans="1:4">
       <c r="A1747" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B1747" t="s">
         <v>646</v>
@@ -26873,7 +26885,7 @@
     </row>
     <row r="1748" spans="1:4">
       <c r="A1748" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B1748" t="s">
         <v>646</v>
@@ -26882,6 +26894,34 @@
         <v>647</v>
       </c>
       <c r="D1748" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:4">
+      <c r="A1749" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1749" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1749" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1749" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:4">
+      <c r="A1750" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1750" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1750" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1750" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added templates for address lines (#228)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1F5D6F-AEEF-4B2A-A358-D97623743B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E622F0E-CE90-40B5-AE3C-0DC534EC9E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7000" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="668">
   <si>
     <t>lang_code</t>
   </si>
@@ -2014,6 +2014,24 @@
   </si>
   <si>
     <t>Photo</t>
+  </si>
+  <si>
+    <t>mosip.address.line1.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.line2.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.line3.template.property</t>
+  </si>
+  <si>
+    <t>Address line1</t>
+  </si>
+  <si>
+    <t>Address line2</t>
+  </si>
+  <si>
+    <t>Address line3</t>
   </si>
 </sst>
 </file>
@@ -2412,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1750"/>
+  <dimension ref="A1:D1753"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1716" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1720" sqref="C1720"/>
+    <sheetView tabSelected="1" topLeftCell="A1710" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1716" sqref="C1716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26412,10 +26430,10 @@
         <v>4</v>
       </c>
       <c r="B1714" t="s">
-        <v>648</v>
+        <v>662</v>
       </c>
       <c r="C1714" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="D1714" s="1" t="s">
         <v>7</v>
@@ -26426,10 +26444,10 @@
         <v>4</v>
       </c>
       <c r="B1715" t="s">
-        <v>649</v>
+        <v>663</v>
       </c>
       <c r="C1715" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="D1715" s="1" t="s">
         <v>7</v>
@@ -26440,10 +26458,10 @@
         <v>4</v>
       </c>
       <c r="B1716" t="s">
-        <v>650</v>
+        <v>664</v>
       </c>
       <c r="C1716" t="s">
-        <v>655</v>
+        <v>667</v>
       </c>
       <c r="D1716" s="1" t="s">
         <v>7</v>
@@ -26454,10 +26472,10 @@
         <v>4</v>
       </c>
       <c r="B1717" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C1717" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D1717" s="1" t="s">
         <v>7</v>
@@ -26468,10 +26486,10 @@
         <v>4</v>
       </c>
       <c r="B1718" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C1718" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D1718" s="1" t="s">
         <v>7</v>
@@ -26482,10 +26500,10 @@
         <v>4</v>
       </c>
       <c r="B1719" t="s">
-        <v>611</v>
+        <v>650</v>
       </c>
       <c r="C1719" t="s">
-        <v>619</v>
+        <v>655</v>
       </c>
       <c r="D1719" s="1" t="s">
         <v>7</v>
@@ -26496,10 +26514,10 @@
         <v>4</v>
       </c>
       <c r="B1720" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="C1720" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="D1720" s="1" t="s">
         <v>7</v>
@@ -26510,10 +26528,10 @@
         <v>4</v>
       </c>
       <c r="B1721" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="C1721" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D1721" s="1" t="s">
         <v>7</v>
@@ -26524,10 +26542,10 @@
         <v>4</v>
       </c>
       <c r="B1722" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C1722" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D1722" s="1" t="s">
         <v>7</v>
@@ -26538,10 +26556,10 @@
         <v>4</v>
       </c>
       <c r="B1723" t="s">
-        <v>622</v>
+        <v>660</v>
       </c>
       <c r="C1723" t="s">
-        <v>623</v>
+        <v>661</v>
       </c>
       <c r="D1723" s="1" t="s">
         <v>7</v>
@@ -26552,10 +26570,10 @@
         <v>4</v>
       </c>
       <c r="B1724" t="s">
-        <v>624</v>
+        <v>658</v>
       </c>
       <c r="C1724" t="s">
-        <v>625</v>
+        <v>659</v>
       </c>
       <c r="D1724" s="1" t="s">
         <v>7</v>
@@ -26566,10 +26584,10 @@
         <v>4</v>
       </c>
       <c r="B1725" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="C1725" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="D1725" s="1" t="s">
         <v>7</v>
@@ -26580,10 +26598,10 @@
         <v>4</v>
       </c>
       <c r="B1726" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="C1726" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="D1726" s="1" t="s">
         <v>7</v>
@@ -26594,10 +26612,10 @@
         <v>4</v>
       </c>
       <c r="B1727" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C1727" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="D1727" s="1" t="s">
         <v>7</v>
@@ -26608,10 +26626,10 @@
         <v>4</v>
       </c>
       <c r="B1728" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="C1728" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="D1728" s="1" t="s">
         <v>7</v>
@@ -26622,10 +26640,10 @@
         <v>4</v>
       </c>
       <c r="B1729" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C1729" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="D1729" s="1" t="s">
         <v>7</v>
@@ -26636,10 +26654,10 @@
         <v>4</v>
       </c>
       <c r="B1730" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="C1730" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="D1730" s="1" t="s">
         <v>7</v>
@@ -26650,10 +26668,10 @@
         <v>4</v>
       </c>
       <c r="B1731" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="C1731" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D1731" s="1" t="s">
         <v>7</v>
@@ -26664,10 +26682,10 @@
         <v>4</v>
       </c>
       <c r="B1732" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="C1732" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="D1732" s="1" t="s">
         <v>7</v>
@@ -26678,10 +26696,10 @@
         <v>4</v>
       </c>
       <c r="B1733" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="C1733" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="D1733" s="1" t="s">
         <v>7</v>
@@ -26692,10 +26710,10 @@
         <v>4</v>
       </c>
       <c r="B1734" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="C1734" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="D1734" s="1" t="s">
         <v>7</v>
@@ -26703,13 +26721,13 @@
     </row>
     <row r="1735" spans="1:4">
       <c r="A1735" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1735" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C1735" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D1735" s="1" t="s">
         <v>7</v>
@@ -26717,13 +26735,13 @@
     </row>
     <row r="1736" spans="1:4">
       <c r="A1736" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1736" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1736" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1736" s="1" t="s">
         <v>7</v>
@@ -26731,13 +26749,13 @@
     </row>
     <row r="1737" spans="1:4">
       <c r="A1737" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B1737" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1737" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1737" s="1" t="s">
         <v>7</v>
@@ -26745,13 +26763,13 @@
     </row>
     <row r="1738" spans="1:4">
       <c r="A1738" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B1738" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1738" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1738" s="1" t="s">
         <v>7</v>
@@ -26759,13 +26777,13 @@
     </row>
     <row r="1739" spans="1:4">
       <c r="A1739" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B1739" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1739" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1739" s="1" t="s">
         <v>7</v>
@@ -26773,13 +26791,13 @@
     </row>
     <row r="1740" spans="1:4">
       <c r="A1740" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B1740" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1740" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1740" s="1" t="s">
         <v>7</v>
@@ -26787,13 +26805,13 @@
     </row>
     <row r="1741" spans="1:4">
       <c r="A1741" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B1741" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1741" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1741" s="1" t="s">
         <v>7</v>
@@ -26801,13 +26819,13 @@
     </row>
     <row r="1742" spans="1:4">
       <c r="A1742" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B1742" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1742" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1742" s="1" t="s">
         <v>7</v>
@@ -26815,13 +26833,13 @@
     </row>
     <row r="1743" spans="1:4">
       <c r="A1743" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B1743" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1743" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1743" s="1" t="s">
         <v>7</v>
@@ -26829,13 +26847,13 @@
     </row>
     <row r="1744" spans="1:4">
       <c r="A1744" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1744" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1744" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1744" s="1" t="s">
         <v>7</v>
@@ -26843,13 +26861,13 @@
     </row>
     <row r="1745" spans="1:4">
       <c r="A1745" t="s">
-        <v>4</v>
+        <v>301</v>
       </c>
       <c r="B1745" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1745" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1745" s="1" t="s">
         <v>7</v>
@@ -26857,13 +26875,13 @@
     </row>
     <row r="1746" spans="1:4">
       <c r="A1746" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B1746" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C1746" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D1746" s="1" t="s">
         <v>7</v>
@@ -26871,13 +26889,13 @@
     </row>
     <row r="1747" spans="1:4">
       <c r="A1747" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B1747" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1747" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1747" s="1" t="s">
         <v>7</v>
@@ -26885,7 +26903,7 @@
     </row>
     <row r="1748" spans="1:4">
       <c r="A1748" t="s">
-        <v>302</v>
+        <v>4</v>
       </c>
       <c r="B1748" t="s">
         <v>646</v>
@@ -26899,7 +26917,7 @@
     </row>
     <row r="1749" spans="1:4">
       <c r="A1749" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B1749" t="s">
         <v>646</v>
@@ -26913,7 +26931,7 @@
     </row>
     <row r="1750" spans="1:4">
       <c r="A1750" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B1750" t="s">
         <v>646</v>
@@ -26922,6 +26940,48 @@
         <v>647</v>
       </c>
       <c r="D1750" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:4">
+      <c r="A1751" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1751" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1751" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:4">
+      <c r="A1752" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1752" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1752" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1752" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:4">
+      <c r="A1753" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1753" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1753" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1753" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new templates for auth-lock-unlock attribute (#229)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E622F0E-CE90-40B5-AE3C-0DC534EC9E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9494A80A-3FC8-490A-AFFC-9AF3F37FB991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="684">
   <si>
     <t>lang_code</t>
   </si>
@@ -2032,6 +2032,54 @@
   </si>
   <si>
     <t>Address line3</t>
+  </si>
+  <si>
+    <t>mosip.otp-email.template.property</t>
+  </si>
+  <si>
+    <t>mosip.otp-phone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.demo.template.property</t>
+  </si>
+  <si>
+    <t>mosip.bio-finger.template.property</t>
+  </si>
+  <si>
+    <t>mosip.bio-iris.template.property</t>
+  </si>
+  <si>
+    <t>mosip.bio-face.template.property</t>
+  </si>
+  <si>
+    <t>Email otp</t>
+  </si>
+  <si>
+    <t>Phone otp</t>
+  </si>
+  <si>
+    <t>Demographic</t>
+  </si>
+  <si>
+    <t>Finger bio</t>
+  </si>
+  <si>
+    <t>Iris bio</t>
+  </si>
+  <si>
+    <t>Face bio</t>
+  </si>
+  <si>
+    <t>mosip.locked.template.property</t>
+  </si>
+  <si>
+    <t>mosip.unlocked.template.property</t>
+  </si>
+  <si>
+    <t>Unlocked status</t>
+  </si>
+  <si>
+    <t>Locked status</t>
   </si>
 </sst>
 </file>
@@ -2430,10 +2478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1753"/>
+  <dimension ref="A1:D1761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1710" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1716" sqref="C1716"/>
+    <sheetView tabSelected="1" topLeftCell="A1752" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1763" sqref="C1763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26985,6 +27033,118 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1754" spans="1:4">
+      <c r="A1754" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1754" t="s">
+        <v>668</v>
+      </c>
+      <c r="C1754" t="s">
+        <v>674</v>
+      </c>
+      <c r="D1754" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:4">
+      <c r="A1755" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1755" t="s">
+        <v>669</v>
+      </c>
+      <c r="C1755" t="s">
+        <v>675</v>
+      </c>
+      <c r="D1755" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:4">
+      <c r="A1756" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1756" t="s">
+        <v>670</v>
+      </c>
+      <c r="C1756" t="s">
+        <v>676</v>
+      </c>
+      <c r="D1756" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:4">
+      <c r="A1757" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1757" t="s">
+        <v>671</v>
+      </c>
+      <c r="C1757" t="s">
+        <v>677</v>
+      </c>
+      <c r="D1757" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:4">
+      <c r="A1758" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1758" t="s">
+        <v>672</v>
+      </c>
+      <c r="C1758" t="s">
+        <v>678</v>
+      </c>
+      <c r="D1758" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:4">
+      <c r="A1759" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1759" t="s">
+        <v>673</v>
+      </c>
+      <c r="C1759" t="s">
+        <v>679</v>
+      </c>
+      <c r="D1759" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:4">
+      <c r="A1760" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1760" t="s">
+        <v>681</v>
+      </c>
+      <c r="C1760" t="s">
+        <v>682</v>
+      </c>
+      <c r="D1760" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:4">
+      <c r="A1761" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1761" t="s">
+        <v>680</v>
+      </c>
+      <c r="C1761" t="s">
+        <v>683</v>
+      </c>
+      <c r="D1761" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
added templates for event status (#253)
* added templates for other languages

* added template type code for different languages

* added spanish language

* fixed code for templates

* updated file format  with spanish language

* added templates for event status
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E92173D-F462-49D4-A0E1-04E09237AA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E8D824-C08A-4C44-9480-149ED5502CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8904" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8988" uniqueCount="691">
   <si>
     <t>lang_code</t>
   </si>
@@ -2078,6 +2078,24 @@
   </si>
   <si>
     <t>spa</t>
+  </si>
+  <si>
+    <t>mosip.event.status.success.template</t>
+  </si>
+  <si>
+    <t>mosip.event.status.failed.template</t>
+  </si>
+  <si>
+    <t>mosip.event.status.inprogress.template</t>
+  </si>
+  <si>
+    <t>Success event status</t>
+  </si>
+  <si>
+    <t>Failed event status</t>
+  </si>
+  <si>
+    <t>In progress event status</t>
   </si>
 </sst>
 </file>
@@ -2497,10 +2515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2226"/>
+  <dimension ref="A1:D2247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2218" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2227" sqref="A2227"/>
+    <sheetView tabSelected="1" topLeftCell="A2235" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2248" sqref="A2248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -33674,6 +33692,300 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2227" spans="1:4">
+      <c r="A2227" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2227" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2227" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2227" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:4">
+      <c r="A2228" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2228" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2228" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2228" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:4">
+      <c r="A2229" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2229" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2229" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2229" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:4">
+      <c r="A2230" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2230" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2230" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2230" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:4">
+      <c r="A2231" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2231" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2231" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2231" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:4">
+      <c r="A2232" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2232" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2232" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2232" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:4">
+      <c r="A2233" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2233" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2233" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2233" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:4">
+      <c r="A2234" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2234" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2234" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2234" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:4">
+      <c r="A2235" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2235" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2235" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2235" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:4">
+      <c r="A2236" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2236" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2236" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2236" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:4">
+      <c r="A2237" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2237" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2237" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2237" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:4">
+      <c r="A2238" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2238" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2238" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2238" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:4">
+      <c r="A2239" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2239" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2239" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2239" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:4">
+      <c r="A2240" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2240" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2240" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2240" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:4">
+      <c r="A2241" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2241" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2241" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2241" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:4">
+      <c r="A2242" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2242" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2242" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2242" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:4">
+      <c r="A2243" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2243" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2243" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2243" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:4">
+      <c r="A2244" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2244" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2244" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2244" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:4">
+      <c r="A2245" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2245" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2245" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2245" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:4">
+      <c r="A2246" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2246" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2246" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2246" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:4">
+      <c r="A2247" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2247" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2247" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2247" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added templates for auth types (#256)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E8D824-C08A-4C44-9480-149ED5502CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AB5609-948E-4530-9863-17363723231D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8988" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9772" uniqueCount="747">
   <si>
     <t>lang_code</t>
   </si>
@@ -2096,6 +2096,174 @@
   </si>
   <si>
     <t>In progress event status</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-REQUEST.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.DEMO-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FINGERPRINT-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IRIS-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FACE-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-STORAGE.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.EKYC-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-EXCHANGE.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IDENTITY-KEY-BINDING.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-REQUEST.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-REQUEST.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.DEMO-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FINGERPRINT-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IRIS-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FACE-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-STORAGE.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.EKYC-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-EXCHANGE.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IDENTITY-KEY-BINDING.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-REQUEST.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-AUTH.N</t>
+  </si>
+  <si>
+    <t>OTP Request Success</t>
+  </si>
+  <si>
+    <t>OTP Authentication Success</t>
+  </si>
+  <si>
+    <t>Demo Authentication Success</t>
+  </si>
+  <si>
+    <t>Finger Authentication Success</t>
+  </si>
+  <si>
+    <t>Iris  Authentication Success</t>
+  </si>
+  <si>
+    <t>Face Authentication Success</t>
+  </si>
+  <si>
+    <t>Pin Authentication Success</t>
+  </si>
+  <si>
+    <t>Static Pin Store Request Success</t>
+  </si>
+  <si>
+    <t>EKYC Authentication Request Success</t>
+  </si>
+  <si>
+    <t>KYC Authentication Request Success</t>
+  </si>
+  <si>
+    <t>KYC Exchange Request Success</t>
+  </si>
+  <si>
+    <t>Identity Key Binding Request Success</t>
+  </si>
+  <si>
+    <t>Token Request Success</t>
+  </si>
+  <si>
+    <t>Token based Authentication Success</t>
+  </si>
+  <si>
+    <t>OTP Request Failed</t>
+  </si>
+  <si>
+    <t>OTP Authentication Failed</t>
+  </si>
+  <si>
+    <t>Demo Authentication Failed</t>
+  </si>
+  <si>
+    <t>Finger Authentication Failed</t>
+  </si>
+  <si>
+    <t>Iris  Authentication Failed</t>
+  </si>
+  <si>
+    <t>Face Authentication Failed</t>
+  </si>
+  <si>
+    <t>Pin Authentication Failed</t>
+  </si>
+  <si>
+    <t>Static Pin Store Request Failed</t>
+  </si>
+  <si>
+    <t>EKYC Authentication Request Failed</t>
+  </si>
+  <si>
+    <t>KYC Authentication Request Failed</t>
+  </si>
+  <si>
+    <t>KYC Exchange Request Failed</t>
+  </si>
+  <si>
+    <t>Identity Key Binding Request Failed</t>
+  </si>
+  <si>
+    <t>Token Request Failed</t>
+  </si>
+  <si>
+    <t>Token based Authentication Failed</t>
   </si>
 </sst>
 </file>
@@ -2515,10 +2683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2247"/>
+  <dimension ref="A1:D2443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2248" sqref="A2248"/>
+    <sheetView tabSelected="1" topLeftCell="A2430" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2444" sqref="A2444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -33986,6 +34154,2750 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2248" spans="1:4">
+      <c r="A2248" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2248" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2248" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2248" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:4">
+      <c r="A2249" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2249" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2249" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2249" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:4">
+      <c r="A2250" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2250" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2250" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2250" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:4">
+      <c r="A2251" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2251" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2251" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2251" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:4">
+      <c r="A2252" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2252" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2252" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2252" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:4">
+      <c r="A2253" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2253" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2253" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2253" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:4">
+      <c r="A2254" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2254" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2254" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2254" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:4">
+      <c r="A2255" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2255" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2255" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2255" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:4">
+      <c r="A2256" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2256" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2256" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2256" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:4">
+      <c r="A2257" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2257" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2257" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2257" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:4">
+      <c r="A2258" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2258" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2258" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2258" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:4">
+      <c r="A2259" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2259" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2259" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2259" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:4">
+      <c r="A2260" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2260" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2260" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2260" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:4">
+      <c r="A2261" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2261" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2261" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2261" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:4">
+      <c r="A2262" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2262" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2262" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2262" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:4">
+      <c r="A2263" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2263" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2263" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2263" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:4">
+      <c r="A2264" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2264" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2264" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2264" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:4">
+      <c r="A2265" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2265" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2265" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2265" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:4">
+      <c r="A2266" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2266" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2266" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2266" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:4">
+      <c r="A2267" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2267" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2267" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2267" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:4">
+      <c r="A2268" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2268" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2268" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2268" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:4">
+      <c r="A2269" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2269" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2269" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2269" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:4">
+      <c r="A2270" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2270" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2270" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2270" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:4">
+      <c r="A2271" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2271" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2271" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2271" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:4">
+      <c r="A2272" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2272" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2272" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2272" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:4">
+      <c r="A2273" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2273" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2273" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2273" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:4">
+      <c r="A2274" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2274" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2274" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2274" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:4">
+      <c r="A2275" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2275" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2275" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2275" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:4">
+      <c r="A2276" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2276" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2276" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2276" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:4">
+      <c r="A2277" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2277" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2277" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2277" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:4">
+      <c r="A2278" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2278" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2278" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2278" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:4">
+      <c r="A2279" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2279" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2279" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2279" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:4">
+      <c r="A2280" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2280" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2280" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2280" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:4">
+      <c r="A2281" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2281" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2281" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2281" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:4">
+      <c r="A2282" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2282" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2282" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2282" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:4">
+      <c r="A2283" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2283" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2283" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2283" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:4">
+      <c r="A2284" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2284" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2284" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2284" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:4">
+      <c r="A2285" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2285" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2285" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2285" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:4">
+      <c r="A2286" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2286" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2286" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2286" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:4">
+      <c r="A2287" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2287" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2287" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2287" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:4">
+      <c r="A2288" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2288" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2288" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2288" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:4">
+      <c r="A2289" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2289" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2289" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2289" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:4">
+      <c r="A2290" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2290" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2290" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2290" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:4">
+      <c r="A2291" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2291" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2291" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2291" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:4">
+      <c r="A2292" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2292" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2292" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2292" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:4">
+      <c r="A2293" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2293" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2293" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2293" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:4">
+      <c r="A2294" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2294" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2294" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2294" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:4">
+      <c r="A2295" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2295" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2295" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2295" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:4">
+      <c r="A2296" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2296" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2296" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2296" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:4">
+      <c r="A2297" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2297" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2297" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2297" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:4">
+      <c r="A2298" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2298" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2298" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2298" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:4">
+      <c r="A2299" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2299" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2299" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2299" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:4">
+      <c r="A2300" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2300" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2300" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2300" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:4">
+      <c r="A2301" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2301" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2301" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2301" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:4">
+      <c r="A2302" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2302" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2302" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2302" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:4">
+      <c r="A2303" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2303" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2303" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2303" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:4">
+      <c r="A2304" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2304" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2304" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2304" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:4">
+      <c r="A2305" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2305" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2305" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2305" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:4">
+      <c r="A2306" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2306" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2306" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2306" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:4">
+      <c r="A2307" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2307" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2307" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2307" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:4">
+      <c r="A2308" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2308" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2308" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2308" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:4">
+      <c r="A2309" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2309" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2309" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2309" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:4">
+      <c r="A2310" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2310" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2310" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2310" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:4">
+      <c r="A2311" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2311" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2311" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2311" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:4">
+      <c r="A2312" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2312" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2312" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2312" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:4">
+      <c r="A2313" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2313" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2313" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2313" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:4">
+      <c r="A2314" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2314" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2314" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2314" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:4">
+      <c r="A2315" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2315" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2315" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2315" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:4">
+      <c r="A2316" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2316" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2316" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2316" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:4">
+      <c r="A2317" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2317" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2317" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2317" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:4">
+      <c r="A2318" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2318" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2318" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2318" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:4">
+      <c r="A2319" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2319" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2319" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2319" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:4">
+      <c r="A2320" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2320" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2320" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2320" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:4">
+      <c r="A2321" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2321" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2321" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2321" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:4">
+      <c r="A2322" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2322" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2322" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2322" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:4">
+      <c r="A2323" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2323" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2323" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2323" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:4">
+      <c r="A2324" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2324" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2324" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2324" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:4">
+      <c r="A2325" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2325" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2325" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2325" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:4">
+      <c r="A2326" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2326" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2326" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2326" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:4">
+      <c r="A2327" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2327" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2327" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2327" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:4">
+      <c r="A2328" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2328" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2328" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2328" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:4">
+      <c r="A2329" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2329" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2329" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2329" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:4">
+      <c r="A2330" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2330" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2330" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2330" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:4">
+      <c r="A2331" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2331" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2331" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2331" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:4">
+      <c r="A2332" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2332" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2332" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2332" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:4">
+      <c r="A2333" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2333" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2333" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2333" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:4">
+      <c r="A2334" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2334" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2334" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2334" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:4">
+      <c r="A2335" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2335" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2335" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2335" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:4">
+      <c r="A2336" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2336" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2336" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2336" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:4">
+      <c r="A2337" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2337" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2337" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2337" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:4">
+      <c r="A2338" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2338" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2338" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2338" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:4">
+      <c r="A2339" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2339" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2339" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2339" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:4">
+      <c r="A2340" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2340" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2340" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2340" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:4">
+      <c r="A2341" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2341" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2341" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2341" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:4">
+      <c r="A2342" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2342" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2342" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2342" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:4">
+      <c r="A2343" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2343" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2343" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2343" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:4">
+      <c r="A2344" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2344" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2344" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2344" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:4">
+      <c r="A2345" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2345" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2345" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2345" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:4">
+      <c r="A2346" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2346" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2346" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2346" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:4">
+      <c r="A2347" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2347" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2347" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2347" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:4">
+      <c r="A2348" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2348" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2348" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2348" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:4">
+      <c r="A2349" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2349" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2349" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2349" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:4">
+      <c r="A2350" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2350" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2350" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2350" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:4">
+      <c r="A2351" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2351" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2351" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2351" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:4">
+      <c r="A2352" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2352" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2352" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2352" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:4">
+      <c r="A2353" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2353" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2353" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2353" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:4">
+      <c r="A2354" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2354" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2354" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2354" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:4">
+      <c r="A2355" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2355" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2355" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2355" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:4">
+      <c r="A2356" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2356" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2356" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2356" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:4">
+      <c r="A2357" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2357" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2357" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2357" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:4">
+      <c r="A2358" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2358" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2358" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2358" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:4">
+      <c r="A2359" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2359" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2359" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2359" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:4">
+      <c r="A2360" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2360" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2360" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2360" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:4">
+      <c r="A2361" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2361" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2361" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2361" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:4">
+      <c r="A2362" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2362" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2362" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2362" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:4">
+      <c r="A2363" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2363" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2363" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2363" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:4">
+      <c r="A2364" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2364" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2364" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2364" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:4">
+      <c r="A2365" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2365" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2365" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2365" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:4">
+      <c r="A2366" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2366" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2366" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2366" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:4">
+      <c r="A2367" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2367" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2367" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2367" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:4">
+      <c r="A2368" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2368" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2368" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2368" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:4">
+      <c r="A2369" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2369" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2369" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2369" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:4">
+      <c r="A2370" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2370" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2370" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2370" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:4">
+      <c r="A2371" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2371" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2371" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2371" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:4">
+      <c r="A2372" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2372" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2372" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2372" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:4">
+      <c r="A2373" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2373" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2373" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2373" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:4">
+      <c r="A2374" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2374" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2374" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2374" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:4">
+      <c r="A2375" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2375" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2375" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2375" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:4">
+      <c r="A2376" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2376" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2376" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2376" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:4">
+      <c r="A2377" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2377" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2377" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2377" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:4">
+      <c r="A2378" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2378" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2378" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2378" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:4">
+      <c r="A2379" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2379" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2379" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2379" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:4">
+      <c r="A2380" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2380" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2380" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2380" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:4">
+      <c r="A2381" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2381" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2381" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2381" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:4">
+      <c r="A2382" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2382" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2382" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2382" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:4">
+      <c r="A2383" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2383" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2383" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2383" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:4">
+      <c r="A2384" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2384" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2384" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2384" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:4">
+      <c r="A2385" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2385" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2385" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2385" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:4">
+      <c r="A2386" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2386" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2386" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2386" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:4">
+      <c r="A2387" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2387" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2387" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2387" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:4">
+      <c r="A2388" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2388" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2388" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2388" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:4">
+      <c r="A2389" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2389" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2389" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2389" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:4">
+      <c r="A2390" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2390" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2390" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2390" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:4">
+      <c r="A2391" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2391" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2391" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2391" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:4">
+      <c r="A2392" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2392" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2392" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2392" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:4">
+      <c r="A2393" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2393" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2393" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2393" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:4">
+      <c r="A2394" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2394" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2394" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2394" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:4">
+      <c r="A2395" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2395" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2395" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2395" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:4">
+      <c r="A2396" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2396" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2396" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2396" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:4">
+      <c r="A2397" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2397" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2397" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2397" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:4">
+      <c r="A2398" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2398" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2398" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2398" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:4">
+      <c r="A2399" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2399" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2399" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2399" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:4">
+      <c r="A2400" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2400" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2400" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2400" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:4">
+      <c r="A2401" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2401" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2401" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2401" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:4">
+      <c r="A2402" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2402" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2402" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2402" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:4">
+      <c r="A2403" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2403" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2403" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2403" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:4">
+      <c r="A2404" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2404" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2404" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2404" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:4">
+      <c r="A2405" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2405" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2405" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2405" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:4">
+      <c r="A2406" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2406" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2406" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2406" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:4">
+      <c r="A2407" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2407" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2407" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2407" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:4">
+      <c r="A2408" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2408" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2408" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2408" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:4">
+      <c r="A2409" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2409" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2409" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2409" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:4">
+      <c r="A2410" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2410" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2410" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2410" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:4">
+      <c r="A2411" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2411" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2411" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2411" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:4">
+      <c r="A2412" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2412" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2412" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2412" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:4">
+      <c r="A2413" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2413" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2413" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2413" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:4">
+      <c r="A2414" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2414" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2414" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2414" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:4">
+      <c r="A2415" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2415" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2415" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2415" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:4">
+      <c r="A2416" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2416" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2416" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2416" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:4">
+      <c r="A2417" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2417" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2417" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2417" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:4">
+      <c r="A2418" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2418" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2418" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2418" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:4">
+      <c r="A2419" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2419" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2419" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2419" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:4">
+      <c r="A2420" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2420" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2420" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2420" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:4">
+      <c r="A2421" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2421" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2421" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2421" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:4">
+      <c r="A2422" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2422" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2422" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2422" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:4">
+      <c r="A2423" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2423" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2423" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2423" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:4">
+      <c r="A2424" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2424" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2424" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2424" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:4">
+      <c r="A2425" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2425" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2425" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2425" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:4">
+      <c r="A2426" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2426" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2426" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2426" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:4">
+      <c r="A2427" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2427" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2427" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2427" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:4">
+      <c r="A2428" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2428" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2428" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2428" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:4">
+      <c r="A2429" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2429" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2429" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2429" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:4">
+      <c r="A2430" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2430" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2430" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2430" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:4">
+      <c r="A2431" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2431" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2431" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2431" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:4">
+      <c r="A2432" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2432" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2432" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2432" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:4">
+      <c r="A2433" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2433" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2433" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2433" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:4">
+      <c r="A2434" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2434" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2434" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2434" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:4">
+      <c r="A2435" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2435" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2435" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2435" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:4">
+      <c r="A2436" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2436" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2436" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2436" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:4">
+      <c r="A2437" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2437" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2437" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2437" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:4">
+      <c r="A2438" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2438" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2438" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2438" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:4">
+      <c r="A2439" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2439" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2439" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2439" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:4">
+      <c r="A2440" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2440" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2440" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2440" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:4">
+      <c r="A2441" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2441" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2441" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2441" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:4">
+      <c r="A2442" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2442" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2442" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2442" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:4">
+      <c r="A2443" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2443" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2443" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2443" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added templates for event types (#259)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB47532A-C573-4679-B035-A1344A948F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9686E3A6-2E78-4136-89FD-57B1FCDF1DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10388" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10780" uniqueCount="818">
   <si>
     <t>lang_code</t>
   </si>
@@ -2393,6 +2393,90 @@
   </si>
   <si>
     <t>mosip.auth-type-code.UNKNOWN</t>
+  </si>
+  <si>
+    <t>Authentication Request event type</t>
+  </si>
+  <si>
+    <t>Share Credential With Partner event type</t>
+  </si>
+  <si>
+    <t>Download Personalized Card event type</t>
+  </si>
+  <si>
+    <t>Order a Physical Card event type</t>
+  </si>
+  <si>
+    <t>Get UIN Card event type</t>
+  </si>
+  <si>
+    <t>Book An Appointment event type</t>
+  </si>
+  <si>
+    <t>Update UIN Data event type</t>
+  </si>
+  <si>
+    <t>Generate VID event type</t>
+  </si>
+  <si>
+    <t>Revoke VID event type</t>
+  </si>
+  <si>
+    <t>Secure My ID event type</t>
+  </si>
+  <si>
+    <t>Download VID Card event type</t>
+  </si>
+  <si>
+    <t>Send OTP event type</t>
+  </si>
+  <si>
+    <t>Verify My Phone/Email event type</t>
+  </si>
+  <si>
+    <t>Default event type</t>
+  </si>
+  <si>
+    <t>mosip.event.type.AUTHENTICATION_REQUEST</t>
+  </si>
+  <si>
+    <t>mosip.event.type.SHARE_CRED_WITH_PARTNER</t>
+  </si>
+  <si>
+    <t>mosip.event.type.DOWNLOAD_PERSONALIZED_CARD</t>
+  </si>
+  <si>
+    <t>mosip.event.type.ORDER_PHYSICAL_CARD</t>
+  </si>
+  <si>
+    <t>mosip.event.type.GET_MY_ID</t>
+  </si>
+  <si>
+    <t>mosip.event.type.BOOK_AN_APPOINTMENT</t>
+  </si>
+  <si>
+    <t>mosip.event.type.UPDATE_MY_UIN</t>
+  </si>
+  <si>
+    <t>mosip.event.type.GENERATE_VID</t>
+  </si>
+  <si>
+    <t>mosip.event.type.REVOKE_VID</t>
+  </si>
+  <si>
+    <t>mosip.event.type.AUTH_TYPE_LOCK_UNLOCK</t>
+  </si>
+  <si>
+    <t>mosip.event.type.VID_CARD_DOWNLOAD</t>
+  </si>
+  <si>
+    <t>mosip.event.type.SEND_OTP</t>
+  </si>
+  <si>
+    <t>mosip.event.type.VALIDATE_OTP</t>
+  </si>
+  <si>
+    <t>mosip.event.type.DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -2812,10 +2896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2597"/>
+  <dimension ref="A1:D2695"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2589" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2598" sqref="A2598"/>
+    <sheetView tabSelected="1" topLeftCell="A2687" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2696" sqref="A2696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -39183,6 +39267,1378 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2598" spans="1:4">
+      <c r="A2598" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2598" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2598" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2598" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:4">
+      <c r="A2599" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2599" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2599" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2599" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:4">
+      <c r="A2600" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2600" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2600" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2600" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:4">
+      <c r="A2601" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2601" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2601" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2601" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:4">
+      <c r="A2602" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2602" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2602" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2602" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:4">
+      <c r="A2603" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2603" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2603" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2603" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:4">
+      <c r="A2604" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2604" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2604" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2604" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:4">
+      <c r="A2605" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2605" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2605" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2605" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:4">
+      <c r="A2606" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2606" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2606" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2606" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:4">
+      <c r="A2607" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2607" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2607" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2607" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:4">
+      <c r="A2608" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2608" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2608" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2608" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:4">
+      <c r="A2609" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2609" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2609" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2609" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:4">
+      <c r="A2610" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2610" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2610" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2610" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:4">
+      <c r="A2611" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2611" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2611" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2611" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:4">
+      <c r="A2612" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2612" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2612" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2612" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:4">
+      <c r="A2613" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2613" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2613" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2613" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:4">
+      <c r="A2614" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2614" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2614" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2614" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:4">
+      <c r="A2615" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2615" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2615" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2615" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:4">
+      <c r="A2616" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2616" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2616" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2616" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:4">
+      <c r="A2617" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2617" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2617" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2617" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:4">
+      <c r="A2618" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2618" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2618" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2618" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:4">
+      <c r="A2619" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2619" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2619" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2619" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:4">
+      <c r="A2620" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2620" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2620" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2620" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:4">
+      <c r="A2621" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2621" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2621" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2621" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:4">
+      <c r="A2622" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2622" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2622" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2622" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:4">
+      <c r="A2623" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2623" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2623" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2623" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:4">
+      <c r="A2624" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2624" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2624" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2624" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:4">
+      <c r="A2625" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2625" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2625" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2625" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:4">
+      <c r="A2626" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2626" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2626" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2626" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:4">
+      <c r="A2627" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2627" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2627" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2627" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:4">
+      <c r="A2628" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2628" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2628" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2628" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:4">
+      <c r="A2629" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2629" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2629" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2629" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:4">
+      <c r="A2630" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2630" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2630" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2630" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:4">
+      <c r="A2631" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2631" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2631" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2631" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:4">
+      <c r="A2632" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2632" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2632" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2632" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:4">
+      <c r="A2633" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2633" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2633" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2633" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:4">
+      <c r="A2634" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2634" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2634" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2634" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:4">
+      <c r="A2635" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2635" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2635" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2635" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:4">
+      <c r="A2636" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2636" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2636" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2636" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:4">
+      <c r="A2637" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2637" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2637" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2637" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:4">
+      <c r="A2638" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2638" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2638" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2638" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:4">
+      <c r="A2639" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2639" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2639" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2639" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:4">
+      <c r="A2640" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2640" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2640" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2640" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:4">
+      <c r="A2641" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2641" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2641" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2641" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:4">
+      <c r="A2642" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2642" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2642" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2642" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:4">
+      <c r="A2643" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2643" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2643" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2643" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:4">
+      <c r="A2644" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2644" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2644" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2644" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:4">
+      <c r="A2645" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2645" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2645" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2645" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:4">
+      <c r="A2646" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2646" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2646" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2646" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:4">
+      <c r="A2647" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2647" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2647" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2647" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:4">
+      <c r="A2648" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2648" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2648" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2648" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:4">
+      <c r="A2649" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2649" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2649" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2649" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:4">
+      <c r="A2650" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2650" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2650" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2650" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:4">
+      <c r="A2651" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2651" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2651" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2651" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:4">
+      <c r="A2652" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2652" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2652" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2652" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:4">
+      <c r="A2653" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2653" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2653" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2653" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:4">
+      <c r="A2654" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2654" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2654" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2654" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:4">
+      <c r="A2655" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2655" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2655" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2655" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:4">
+      <c r="A2656" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2656" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2656" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2656" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:4">
+      <c r="A2657" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2657" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2657" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2657" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:4">
+      <c r="A2658" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2658" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2658" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2658" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:4">
+      <c r="A2659" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2659" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2659" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2659" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:4">
+      <c r="A2660" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2660" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2660" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2660" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:4">
+      <c r="A2661" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2661" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2661" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2661" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:4">
+      <c r="A2662" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2662" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2662" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2662" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:4">
+      <c r="A2663" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2663" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2663" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2663" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:4">
+      <c r="A2664" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2664" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2664" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2664" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:4">
+      <c r="A2665" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2665" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2665" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2665" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:4">
+      <c r="A2666" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2666" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2666" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2666" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:4">
+      <c r="A2667" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2667" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2667" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2667" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:4">
+      <c r="A2668" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2668" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2668" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2668" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:4">
+      <c r="A2669" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2669" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2669" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2669" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:4">
+      <c r="A2670" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2670" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2670" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2670" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:4">
+      <c r="A2671" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2671" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2671" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2671" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:4">
+      <c r="A2672" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2672" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2672" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2672" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:4">
+      <c r="A2673" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2673" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2673" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2673" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:4">
+      <c r="A2674" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2674" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2674" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2674" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:4">
+      <c r="A2675" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2675" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2675" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2675" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:4">
+      <c r="A2676" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2676" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2676" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2676" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:4">
+      <c r="A2677" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2677" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2677" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2677" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:4">
+      <c r="A2678" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2678" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2678" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2678" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:4">
+      <c r="A2679" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2679" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2679" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2679" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:4">
+      <c r="A2680" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2680" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2680" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2680" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:4">
+      <c r="A2681" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2681" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2681" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2681" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:4">
+      <c r="A2682" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2682" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2682" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2682" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:4">
+      <c r="A2683" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2683" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2683" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2683" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:4">
+      <c r="A2684" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2684" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2684" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2684" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:4">
+      <c r="A2685" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2685" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2685" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2685" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:4">
+      <c r="A2686" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2686" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2686" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2686" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:4">
+      <c r="A2687" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2687" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2687" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2687" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:4">
+      <c r="A2688" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2688" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2688" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2688" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:4">
+      <c r="A2689" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2689" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2689" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2689" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:4">
+      <c r="A2690" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2690" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2690" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2690" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:4">
+      <c r="A2691" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2691" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2691" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2691" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:4">
+      <c r="A2692" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2692" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2692" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2692" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:4">
+      <c r="A2693" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2693" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2693" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2693" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:4">
+      <c r="A2694" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2694" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2694" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2694" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:4">
+      <c r="A2695" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2695" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2695" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2695" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added templates for generate revoke msg (#263)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5B0F94-DE08-4F06-9012-ECBBD5913697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35702D44-441F-4065-9FC9-1FCAC9389F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9548" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9604" uniqueCount="735">
   <si>
     <t>lang_code</t>
   </si>
@@ -2216,6 +2216,18 @@
   </si>
   <si>
     <t>Unknown attribute</t>
+  </si>
+  <si>
+    <t>mosip.generated.template.property</t>
+  </si>
+  <si>
+    <t>mosip.revoked.template.property</t>
+  </si>
+  <si>
+    <t>Generated</t>
+  </si>
+  <si>
+    <t>Revoked</t>
   </si>
 </sst>
 </file>
@@ -2622,10 +2634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2387"/>
+  <dimension ref="A1:D2401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2380" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2388" sqref="A2388"/>
+    <sheetView tabSelected="1" topLeftCell="A2386" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2402" sqref="A2402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -36053,6 +36065,202 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2388" spans="1:4">
+      <c r="A2388" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2388" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2388" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2388" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:4">
+      <c r="A2389" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2389" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2389" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2389" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:4">
+      <c r="A2390" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2390" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2390" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2390" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:4">
+      <c r="A2391" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2391" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2391" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2391" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:4">
+      <c r="A2392" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2392" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2392" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2392" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:4">
+      <c r="A2393" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2393" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2393" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2393" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:4">
+      <c r="A2394" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2394" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2394" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2394" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:4">
+      <c r="A2395" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2395" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2395" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2395" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:4">
+      <c r="A2396" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2396" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2396" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2396" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:4">
+      <c r="A2397" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2397" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2397" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2397" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:4">
+      <c r="A2398" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2398" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2398" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2398" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:4">
+      <c r="A2399" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2399" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2399" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2399" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:4">
+      <c r="A2400" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2400" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2400" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2400" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:4">
+      <c r="A2401" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2401" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2401" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2401" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-31877 Add template for resident notification in eng
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35702D44-441F-4065-9FC9-1FCAC9389F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22719CDE-D2F5-4074-AA02-3F1151F68632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9604" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9628" uniqueCount="741">
   <si>
     <t>lang_code</t>
   </si>
@@ -2228,6 +2228,24 @@
   </si>
   <si>
     <t>Revoked</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-success-email-subject</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-success-email-content</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-failure-email-subject</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-failure-email-content</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-success_SMS</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-failure_SMS</t>
   </si>
 </sst>
 </file>
@@ -2634,17 +2652,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2401"/>
+  <dimension ref="A1:D2407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2386" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2402" sqref="A2402"/>
+    <sheetView tabSelected="1" topLeftCell="A2395" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2407" sqref="C2407"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.54296875" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1"/>
+    <col min="4" max="4" width="8.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -36261,6 +36279,90 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2402" spans="1:4">
+      <c r="A2402" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2402" t="s">
+        <v>735</v>
+      </c>
+      <c r="C2402" t="s">
+        <v>547</v>
+      </c>
+      <c r="D2402" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:4">
+      <c r="A2403" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2403" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2403" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2403" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:4">
+      <c r="A2404" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2404" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2404" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2404" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:4">
+      <c r="A2405" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2405" t="s">
+        <v>738</v>
+      </c>
+      <c r="C2405" t="s">
+        <v>551</v>
+      </c>
+      <c r="D2405" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:4">
+      <c r="A2406" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2406" t="s">
+        <v>739</v>
+      </c>
+      <c r="C2406" t="s">
+        <v>583</v>
+      </c>
+      <c r="D2406" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:4">
+      <c r="A2407" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2407" t="s">
+        <v>740</v>
+      </c>
+      <c r="C2407" t="s">
+        <v>584</v>
+      </c>
+      <c r="D2407" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-31877 Added all lang data for update-demo-data-regproc-success-email-content
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C7BC4D-4F41-4542-94FF-9D22939292DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB377E25-DCD2-4111-BBAB-117A8757C0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9652" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9676" uniqueCount="741">
   <si>
     <t>lang_code</t>
   </si>
@@ -2663,10 +2663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2413"/>
+  <dimension ref="A1:D2419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2399" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2414" sqref="C2414"/>
+    <sheetView tabSelected="1" topLeftCell="A2402" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2414" sqref="A2414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -36458,6 +36458,90 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2414" spans="1:4">
+      <c r="A2414" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2414" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2414" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2414" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:4">
+      <c r="A2415" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2415" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2415" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2415" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:4">
+      <c r="A2416" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2416" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2416" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2416" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:4">
+      <c r="A2417" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2417" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2417" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2417" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:4">
+      <c r="A2418" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2418" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2418" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2418" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:4">
+      <c r="A2419" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2419" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2419" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2419" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-31877 Added all lang data for update-demo-data-regproc-failure-email-subject
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB377E25-DCD2-4111-BBAB-117A8757C0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE12F88-A6BF-490C-A27D-08BF2468D7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9676" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9700" uniqueCount="741">
   <si>
     <t>lang_code</t>
   </si>
@@ -2663,10 +2663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2419"/>
+  <dimension ref="A1:D2425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2402" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2414" sqref="A2414"/>
+    <sheetView tabSelected="1" topLeftCell="A2411" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2420" sqref="B2420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -36542,6 +36542,90 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2420" spans="1:4">
+      <c r="A2420" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2420" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2420" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2420" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:4">
+      <c r="A2421" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2421" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2421" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2421" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:4">
+      <c r="A2422" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2422" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2422" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2422" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:4">
+      <c r="A2423" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2423" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2423" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2423" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:4">
+      <c r="A2424" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2424" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2424" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2424" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:4">
+      <c r="A2425" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2425" t="s">
+        <v>737</v>
+      </c>
+      <c r="C2425" t="s">
+        <v>548</v>
+      </c>
+      <c r="D2425" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-31877 Added template for discard draft in eng
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0974F11B-E2AA-41D4-ACF6-CEB71D8D84AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170CF29A-70C3-4C55-8016-B5D230BEF04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9772" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9784" uniqueCount="747">
   <si>
     <t>lang_code</t>
   </si>
@@ -2257,6 +2257,24 @@
   </si>
   <si>
     <t>update-demo-data-regproc-failure_SMS</t>
+  </si>
+  <si>
+    <t>update-demo-data-discarded-email-subject</t>
+  </si>
+  <si>
+    <t>update-demo-data-discarded-email-content</t>
+  </si>
+  <si>
+    <t>update-demo-data-discarded-SMS</t>
+  </si>
+  <si>
+    <t>Failure email subject to Discard draft</t>
+  </si>
+  <si>
+    <t>Failure email content to Discard draft</t>
+  </si>
+  <si>
+    <t>Failure SMS content to discard draft</t>
   </si>
 </sst>
 </file>
@@ -2663,10 +2681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2443"/>
+  <dimension ref="A1:D2446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2432" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2441" sqref="B2441"/>
+    <sheetView tabSelected="1" topLeftCell="A2438" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2444" sqref="B2444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -36878,6 +36896,48 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2444" spans="1:4">
+      <c r="A2444" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2444" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2444" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2444" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:4">
+      <c r="A2445" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2445" t="s">
+        <v>742</v>
+      </c>
+      <c r="C2445" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2445" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:4">
+      <c r="A2446" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2446" t="s">
+        <v>743</v>
+      </c>
+      <c r="C2446" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2446" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-31877 Added template for discard draft
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170CF29A-70C3-4C55-8016-B5D230BEF04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33CE4B4-76A9-4625-AC99-2506C65D9007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9784" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9856" uniqueCount="747">
   <si>
     <t>lang_code</t>
   </si>
@@ -2681,10 +2681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2446"/>
+  <dimension ref="A1:D2464"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2438" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2444" sqref="B2444"/>
+    <sheetView tabSelected="1" topLeftCell="A2450" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2462" sqref="C2462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -36938,6 +36938,258 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2447" spans="1:4">
+      <c r="A2447" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2447" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2447" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2447" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:4">
+      <c r="A2448" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2448" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2448" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2448" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:4">
+      <c r="A2449" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2449" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2449" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2449" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:4">
+      <c r="A2450" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2450" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2450" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2450" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:4">
+      <c r="A2451" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2451" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2451" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2451" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:4">
+      <c r="A2452" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2452" t="s">
+        <v>741</v>
+      </c>
+      <c r="C2452" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2452" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:4">
+      <c r="A2453" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2453" t="s">
+        <v>742</v>
+      </c>
+      <c r="C2453" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2453" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:4">
+      <c r="A2454" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2454" t="s">
+        <v>742</v>
+      </c>
+      <c r="C2454" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2454" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:4">
+      <c r="A2455" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2455" t="s">
+        <v>742</v>
+      </c>
+      <c r="C2455" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2455" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:4">
+      <c r="A2456" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2456" t="s">
+        <v>742</v>
+      </c>
+      <c r="C2456" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2456" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:4">
+      <c r="A2457" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2457" t="s">
+        <v>742</v>
+      </c>
+      <c r="C2457" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2457" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:4">
+      <c r="A2458" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2458" t="s">
+        <v>742</v>
+      </c>
+      <c r="C2458" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2458" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:4">
+      <c r="A2459" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2459" t="s">
+        <v>743</v>
+      </c>
+      <c r="C2459" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2459" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:4">
+      <c r="A2460" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2460" t="s">
+        <v>743</v>
+      </c>
+      <c r="C2460" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2460" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:4">
+      <c r="A2461" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2461" t="s">
+        <v>743</v>
+      </c>
+      <c r="C2461" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2461" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:4">
+      <c r="A2462" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2462" t="s">
+        <v>743</v>
+      </c>
+      <c r="C2462" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2462" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:4">
+      <c r="A2463" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2463" t="s">
+        <v>743</v>
+      </c>
+      <c r="C2463" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2463" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:4">
+      <c r="A2464" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2464" t="s">
+        <v>743</v>
+      </c>
+      <c r="C2464" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2464" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-31877 Added templates for cancelled status code in eng
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33CE4B4-76A9-4625-AC99-2506C65D9007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E2D90B-F132-4429-A7C5-F1C70DFA0757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9856" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9868" uniqueCount="753">
   <si>
     <t>lang_code</t>
   </si>
@@ -2275,13 +2275,31 @@
   </si>
   <si>
     <t>Failure SMS content to discard draft</t>
+  </si>
+  <si>
+    <t>mosip.event.status.cancelled.template</t>
+  </si>
+  <si>
+    <t>Cancelled event status</t>
+  </si>
+  <si>
+    <t>update-demo-data-cancelled-summary</t>
+  </si>
+  <si>
+    <t>Cancelled summary to self update demographic data</t>
+  </si>
+  <si>
+    <t>update-demo-data-cancelled-purpose</t>
+  </si>
+  <si>
+    <t>Cancelled Purpose to self update demographic data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2317,6 +2335,12 @@
       <sz val="10"/>
       <color rgb="FF067D17"/>
       <name val="&quot;JetBrains Mono&quot;"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2356,7 +2380,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2369,6 +2393,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2681,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2464"/>
+  <dimension ref="A1:D2467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2450" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2462" sqref="C2462"/>
+    <sheetView tabSelected="1" topLeftCell="A2461" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2467" sqref="B2467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -17426,7 +17453,7 @@
       <c r="A1053" t="s">
         <v>4</v>
       </c>
-      <c r="B1053" s="4" t="s">
+      <c r="B1053" s="6" t="s">
         <v>436</v>
       </c>
       <c r="C1053" s="4" t="s">
@@ -37187,6 +37214,48 @@
         <v>746</v>
       </c>
       <c r="D2464" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:4">
+      <c r="A2465" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2465" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C2465" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2465" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:4">
+      <c r="A2466" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2466" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2466" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2466" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:4">
+      <c r="A2467" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2467" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2467" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="D2467" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MOSIP-31877 Added templates for canceled type
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E2D90B-F132-4429-A7C5-F1C70DFA0757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A99562-BA93-4A94-AB19-ED912C85305D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9868" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9940" uniqueCount="753">
   <si>
     <t>lang_code</t>
   </si>
@@ -2708,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2467"/>
+  <dimension ref="A1:D2485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2461" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2467" sqref="B2467"/>
+    <sheetView tabSelected="1" topLeftCell="A2470" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2485" sqref="D2485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -37259,6 +37259,258 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2468" spans="1:4">
+      <c r="A2468" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2468" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C2468" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2468" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:4">
+      <c r="A2469" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2469" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C2469" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2469" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:4">
+      <c r="A2470" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2470" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C2470" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2470" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:4">
+      <c r="A2471" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2471" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C2471" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2471" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:4">
+      <c r="A2472" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2472" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C2472" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2472" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:4">
+      <c r="A2473" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2473" s="6" t="s">
+        <v>747</v>
+      </c>
+      <c r="C2473" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2473" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:4">
+      <c r="A2474" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2474" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2474" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2474" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:4">
+      <c r="A2475" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2475" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2475" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2475" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:4">
+      <c r="A2476" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2476" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2476" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2476" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:4">
+      <c r="A2477" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2477" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2477" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2477" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:4">
+      <c r="A2478" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2478" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2478" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2478" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:4">
+      <c r="A2479" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2479" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2479" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2479" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:4">
+      <c r="A2480" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2480" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2480" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2480" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:4">
+      <c r="A2481" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2481" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2481" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2481" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:4">
+      <c r="A2482" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2482" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2482" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2482" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:4">
+      <c r="A2483" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2483" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2483" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2483" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:4">
+      <c r="A2484" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2484" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2484" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2484" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:4">
+      <c r="A2485" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2485" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C2485" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2485" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-32019 Added template for regproc success stage in resident
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A99562-BA93-4A94-AB19-ED912C85305D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CD960A-4691-46E8-8E0B-90712386D159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9940" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9968" uniqueCount="755">
   <si>
     <t>lang_code</t>
   </si>
@@ -2293,13 +2293,19 @@
   </si>
   <si>
     <t>Cancelled Purpose to self update demographic data</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-success-summary</t>
+  </si>
+  <si>
+    <t>Regproc success summary to self update demographic data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2342,6 +2348,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2380,7 +2392,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2397,6 +2409,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2708,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2485"/>
+  <dimension ref="A1:D2492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2470" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2485" sqref="D2485"/>
+    <sheetView tabSelected="1" topLeftCell="A2478" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2486" sqref="A2486:A2492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -37511,6 +37526,104 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2486" spans="1:4">
+      <c r="A2486" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2486" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2486" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2486" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:4">
+      <c r="A2487" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2487" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2487" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2487" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:4">
+      <c r="A2488" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2488" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2488" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2488" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:4">
+      <c r="A2489" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2489" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2489" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2489" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:4">
+      <c r="A2490" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2490" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2490" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2490" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:4">
+      <c r="A2491" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2491" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2491" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2491" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:4">
+      <c r="A2492" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2492" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="C2492" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2492" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-32019 Added template for regproc success stage purpose in resident
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CD960A-4691-46E8-8E0B-90712386D159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4134A0-B6AA-4FD1-953D-5327C209696F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9968" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9996" uniqueCount="756">
   <si>
     <t>lang_code</t>
   </si>
@@ -2299,6 +2299,9 @@
   </si>
   <si>
     <t>Regproc success summary to self update demographic data</t>
+  </si>
+  <si>
+    <t>update-demo-data-regproc-success-purpose</t>
   </si>
 </sst>
 </file>
@@ -2723,10 +2726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2492"/>
+  <dimension ref="A1:D2499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2478" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2486" sqref="A2486:A2492"/>
+    <sheetView tabSelected="1" topLeftCell="A2487" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2493" sqref="B2493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -37624,6 +37627,104 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2493" spans="1:4">
+      <c r="A2493" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2493" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2493" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2493" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:4">
+      <c r="A2494" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2494" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2494" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2494" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:4">
+      <c r="A2495" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2495" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2495" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2495" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:4">
+      <c r="A2496" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2496" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2496" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2496" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:4">
+      <c r="A2497" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2497" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2497" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2497" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:4">
+      <c r="A2498" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2498" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2498" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2498" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:4">
+      <c r="A2499" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2499" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C2499" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="D2499" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
MOSIP-35257 Added missing templates for resident service.
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B7E9E3-6938-48A3-B103-EF9F2177FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FBD232-C82B-47AC-B317-F76556C5A17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14838" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14964" uniqueCount="1399">
   <si>
     <t>lang_code</t>
   </si>
@@ -5820,12 +5820,30 @@
   <si>
     <t>now()</t>
   </si>
+  <si>
+    <t>authentication-request-positive-purpose</t>
+  </si>
+  <si>
+    <t>authentication-request-negative-purpose</t>
+  </si>
+  <si>
+    <t>Authentication negative purpose</t>
+  </si>
+  <si>
+    <t>Authentication positive purpose</t>
+  </si>
+  <si>
+    <t>authentication-request-positive-summary</t>
+  </si>
+  <si>
+    <t>Authentication positive summary</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5856,13 +5874,13 @@
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5880,6 +5898,12 @@
       <sz val="10"/>
       <color rgb="FF067D17"/>
       <name val="&quot;JetBrains Mono&quot;"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5928,7 +5952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5969,6 +5993,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6278,10 +6305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2473"/>
+  <dimension ref="A1:F2494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2454" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2466" sqref="B2466"/>
+    <sheetView tabSelected="1" topLeftCell="A2478" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2493" sqref="B2493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -55752,6 +55779,426 @@
         <v>1392</v>
       </c>
     </row>
+    <row r="2474" spans="1:6">
+      <c r="A2474" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2474" s="19" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C2474" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D2474" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2474" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2474" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:6">
+      <c r="A2475" t="s">
+        <v>557</v>
+      </c>
+      <c r="B2475" s="19" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C2475" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D2475" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2475" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2475" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:6">
+      <c r="A2476" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2476" s="19" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C2476" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D2476" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2476" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2476" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:6">
+      <c r="A2477" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2477" s="19" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C2477" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D2477" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2477" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2477" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:6">
+      <c r="A2478" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2478" s="19" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C2478" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D2478" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2478" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2478" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:6">
+      <c r="A2479" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2479" s="19" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C2479" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D2479" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2479" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2479" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:6">
+      <c r="A2480" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2480" s="19" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C2480" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D2480" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2480" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2480" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:6">
+      <c r="A2481" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2481" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C2481" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D2481" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2481" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2481" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:6">
+      <c r="A2482" t="s">
+        <v>557</v>
+      </c>
+      <c r="B2482" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C2482" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D2482" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2482" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2482" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:6">
+      <c r="A2483" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2483" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C2483" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D2483" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2483" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2483" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:6">
+      <c r="A2484" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2484" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C2484" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D2484" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2484" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2484" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:6">
+      <c r="A2485" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2485" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C2485" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D2485" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2485" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2485" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:6">
+      <c r="A2486" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2486" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C2486" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D2486" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2486" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2486" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:6">
+      <c r="A2487" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2487" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C2487" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D2487" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2487" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2487" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:6">
+      <c r="A2488" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2488" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C2488" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2488" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2488" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2488" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:6">
+      <c r="A2489" t="s">
+        <v>557</v>
+      </c>
+      <c r="B2489" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C2489" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2489" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2489" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2489" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:6">
+      <c r="A2490" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2490" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C2490" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2490" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2490" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2490" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:6">
+      <c r="A2491" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2491" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C2491" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2491" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2491" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2491" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:6">
+      <c r="A2492" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2492" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C2492" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2492" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2492" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2492" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2493" spans="1:6">
+      <c r="A2493" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2493" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C2493" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2493" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2493" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2493" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:6">
+      <c r="A2494" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2494" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C2494" s="7" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D2494" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2494" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2494" t="s">
+        <v>1392</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D365" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
ack slip add in temp excxel
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira-qa\tf-nira-dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FCA463-3D86-4AC6-9C36-CA205CF91E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33851DF8-79A8-437A-8F13-A15097A77F2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7048" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7052" uniqueCount="688">
   <si>
     <t>lang_code</t>
   </si>
@@ -2086,6 +2086,12 @@
   </si>
   <si>
     <t>Registration Client</t>
+  </si>
+  <si>
+    <t>reg_ack_a6slip_template_part1</t>
+  </si>
+  <si>
+    <t>A6 - reg</t>
   </si>
 </sst>
 </file>
@@ -2491,17 +2497,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1762"/>
+  <dimension ref="A1:D1763"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1758" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1763" sqref="C1763"/>
+    <sheetView tabSelected="1" topLeftCell="A1744" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1763" sqref="E1763"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -27169,6 +27175,20 @@
         <v>685</v>
       </c>
       <c r="D1762" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:4">
+      <c r="A1763" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1763" t="s">
+        <v>686</v>
+      </c>
+      <c r="C1763" t="s">
+        <v>687</v>
+      </c>
+      <c r="D1763" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ack slip add in temp excxel (#2)
* ack slip add in temp excxel

* xlsx update
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira-qa\tf-nira-dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FCA463-3D86-4AC6-9C36-CA205CF91E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33851DF8-79A8-437A-8F13-A15097A77F2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7048" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7052" uniqueCount="688">
   <si>
     <t>lang_code</t>
   </si>
@@ -2086,6 +2086,12 @@
   </si>
   <si>
     <t>Registration Client</t>
+  </si>
+  <si>
+    <t>reg_ack_a6slip_template_part1</t>
+  </si>
+  <si>
+    <t>A6 - reg</t>
   </si>
 </sst>
 </file>
@@ -2491,17 +2497,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1762"/>
+  <dimension ref="A1:D1763"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1758" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1763" sqref="C1763"/>
+    <sheetView tabSelected="1" topLeftCell="A1744" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1763" sqref="E1763"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -27169,6 +27175,20 @@
         <v>685</v>
       </c>
       <c r="D1762" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:4">
+      <c r="A1763" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1763" t="s">
+        <v>686</v>
+      </c>
+      <c r="C1763" t="s">
+        <v>687</v>
+      </c>
+      <c r="D1763" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated renewal email and SMS in template type
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira-qa\tf-nira-dev\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33851DF8-79A8-437A-8F13-A15097A77F2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357BF971-88BB-4773-AE69-8C9A38FD449F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7052" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7060" uniqueCount="692">
   <si>
     <t>lang_code</t>
   </si>
@@ -2092,6 +2092,18 @@
   </si>
   <si>
     <t>A6 - reg</t>
+  </si>
+  <si>
+    <t>Renewal-of-Card-Reg-Proc-Notification-Email</t>
+  </si>
+  <si>
+    <t>Renewal of Card Reg Proc Notification Email</t>
+  </si>
+  <si>
+    <t>Renewal-of-Card-Reg-Proc-Notification-Sms</t>
+  </si>
+  <si>
+    <t>Renewal of Card Reg Proc Notification Sms</t>
   </si>
 </sst>
 </file>
@@ -2497,10 +2509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1763"/>
+  <dimension ref="A1:D1765"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1744" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1763" sqref="E1763"/>
+    <sheetView tabSelected="1" topLeftCell="A1748" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1763" sqref="G1763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -27192,6 +27204,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1764" spans="1:4">
+      <c r="A1764" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1764" t="s">
+        <v>688</v>
+      </c>
+      <c r="C1764" t="s">
+        <v>689</v>
+      </c>
+      <c r="D1764" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:4">
+      <c r="A1765" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1765" t="s">
+        <v>690</v>
+      </c>
+      <c r="C1765" t="s">
+        <v>691</v>
+      </c>
+      <c r="D1765" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1761" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Revert "Updated renewal email and SMS in template type"
This reverts commit 39fce79c2aa9b07bcc6236ba1cf0d50ca22ce08c.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira-qa\tf-nira-dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357BF971-88BB-4773-AE69-8C9A38FD449F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33851DF8-79A8-437A-8F13-A15097A77F2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7060" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7052" uniqueCount="688">
   <si>
     <t>lang_code</t>
   </si>
@@ -2092,18 +2092,6 @@
   </si>
   <si>
     <t>A6 - reg</t>
-  </si>
-  <si>
-    <t>Renewal-of-Card-Reg-Proc-Notification-Email</t>
-  </si>
-  <si>
-    <t>Renewal of Card Reg Proc Notification Email</t>
-  </si>
-  <si>
-    <t>Renewal-of-Card-Reg-Proc-Notification-Sms</t>
-  </si>
-  <si>
-    <t>Renewal of Card Reg Proc Notification Sms</t>
   </si>
 </sst>
 </file>
@@ -2509,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1765"/>
+  <dimension ref="A1:D1763"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1748" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1763" sqref="G1763"/>
+    <sheetView tabSelected="1" topLeftCell="A1744" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1763" sqref="E1763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -27204,34 +27192,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1764" spans="1:4">
-      <c r="A1764" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1764" t="s">
-        <v>688</v>
-      </c>
-      <c r="C1764" t="s">
-        <v>689</v>
-      </c>
-      <c r="D1764" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1765" spans="1:4">
-      <c r="A1765" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1765" t="s">
-        <v>690</v>
-      </c>
-      <c r="C1765" t="s">
-        <v>691</v>
-      </c>
-      <c r="D1765" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:D1761" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>